<commit_message>
update tag 5 question
</commit_message>
<xml_diff>
--- a/data/train.xlsx
+++ b/data/train.xlsx
@@ -1185,7 +1185,7 @@
         <v>ห้า</v>
       </c>
       <c r="B104" t="str">
-        <v>กฎหมายเกี่ยวกับการขายของออนไลน์มีไว้ทำไม</v>
+        <v>ร้านขายของออนไลน์แบบไหน ที่ต้องจดทะเบียนพาณิชย์อิเล็กทรอนิกส์</v>
       </c>
     </row>
     <row r="105">
@@ -1193,7 +1193,7 @@
         <v>ห้า</v>
       </c>
       <c r="B105" t="str">
-        <v>กฎหมายการขายของออนไลน์</v>
+        <v>กฎหมายการขายของอิเล็กทรอนิกส์</v>
       </c>
     </row>
     <row r="106">
@@ -1201,7 +1201,7 @@
         <v>ห้า</v>
       </c>
       <c r="B106" t="str">
-        <v>กฎหมายขายของออนไลน์</v>
+        <v>กฎหมายขายของอิเล็กทรอนิกส์</v>
       </c>
     </row>
     <row r="107">
@@ -1209,7 +1209,7 @@
         <v>ห้า</v>
       </c>
       <c r="B107" t="str">
-        <v>กฎหมายควบคุม</v>
+        <v>จดทะเบียนอิเล็กทรอนิกส์</v>
       </c>
     </row>
     <row r="108">
@@ -1217,7 +1217,7 @@
         <v>ห้า</v>
       </c>
       <c r="B108" t="str">
-        <v>กฎหมายควบคุมการขายของออนไลน์</v>
+        <v>อิเล็กทรอนิกส์</v>
       </c>
     </row>
     <row r="109">
@@ -1233,7 +1233,7 @@
         <v>ห้า</v>
       </c>
       <c r="B110" t="str">
-        <v>ประโยชน์ของกฎหมาย</v>
+        <v>ทะเบียนพาณิชย์อิเล็กทรอนิกส์</v>
       </c>
     </row>
     <row r="111">
@@ -1241,7 +1241,7 @@
         <v>ห้า</v>
       </c>
       <c r="B111" t="str">
-        <v>ประโยชน์ของกฎหมายออนไลน์</v>
+        <v>ร้านแบบไหนต้องขดทะเบียนอิเล็กทรอนิกส์</v>
       </c>
     </row>
     <row r="112">
@@ -1249,7 +1249,7 @@
         <v>ห้า</v>
       </c>
       <c r="B112" t="str">
-        <v>ประโยชน์ของกฎหมายการขายของออนไลน์</v>
+        <v xml:space="preserve">ร้านขายของออนไลน์แบบไหน </v>
       </c>
     </row>
     <row r="113">
@@ -1257,7 +1257,7 @@
         <v>ห้า</v>
       </c>
       <c r="B113" t="str">
-        <v>ประโยชน์ของกฎหมายการขายออนไลน์</v>
+        <v>ร้านที่ต้องจดทะเบียนอิเล็กทรอนิกส์</v>
       </c>
     </row>
     <row r="114">
@@ -1265,7 +1265,7 @@
         <v>ห้า</v>
       </c>
       <c r="B114" t="str">
-        <v>ประโยชน์กฎหมาย</v>
+        <v>ทะเบียนพาณิชย์อิเล็กทรอนิกส์</v>
       </c>
     </row>
     <row r="115">
@@ -1273,7 +1273,7 @@
         <v>ห้า</v>
       </c>
       <c r="B115" t="str">
-        <v>ประโยชน์ของกฎหมายควบคุมการขายของออนไลน์</v>
+        <v>จดทะเบียนพาณิชย์อิเล็กทรอนิกส์</v>
       </c>
     </row>
     <row r="116">
@@ -1281,7 +1281,7 @@
         <v>ห้า</v>
       </c>
       <c r="B116" t="str">
-        <v>ประโยชน์ของกฎหมายควบคุมการขายออนไลน์</v>
+        <v>การจดทะเบียนพาณิชย์อิเล็กทรอนิกส์</v>
       </c>
     </row>
     <row r="117">
@@ -1289,7 +1289,7 @@
         <v>ห้า</v>
       </c>
       <c r="B117" t="str">
-        <v>ประโยชน์กฎหมายการขายของออนไลน์</v>
+        <v>การจดทะเบียนอิเล็กทรอนิกส์</v>
       </c>
     </row>
     <row r="118">
@@ -1297,7 +1297,7 @@
         <v>ห้า</v>
       </c>
       <c r="B118" t="str">
-        <v>ประโยชน์กฎหมายการขายออนไลน์</v>
+        <v>DBD Registered</v>
       </c>
     </row>
     <row r="119">
@@ -1305,7 +1305,7 @@
         <v>ห้า</v>
       </c>
       <c r="B119" t="str">
-        <v>ประโยชน์</v>
+        <v>dbd registered</v>
       </c>
     </row>
     <row r="121">

</xml_diff>

<commit_message>
delete unnecessary q and add some more q
</commit_message>
<xml_diff>
--- a/data/train.xlsx
+++ b/data/train.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project_chatbot\chat_bot_team\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F86B60-CCD6-45A5-B387-1B34CE77409C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF8693E5-9E4A-462A-B0F0-561A6F817577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="212">
   <si>
     <t>tag</t>
   </si>
@@ -31,12 +31,6 @@
     <t>หนึ่ง</t>
   </si>
   <si>
-    <t>กฎหมายที่เกี่ยวข้องกับการขายของออนไลน์มีกฎหมายสำคัญๆใดที่เกี่ยวข้องบ้าง</t>
-  </si>
-  <si>
-    <t>กฎหมาย</t>
-  </si>
-  <si>
     <t>กฎหมายขายของออนไลน์</t>
   </si>
   <si>
@@ -91,9 +85,6 @@
     <t>สอง</t>
   </si>
   <si>
-    <t>การแชร์รูปภาพหรือข้อความต่างๆ เกี่ยวกับร้านค้าออนไลน์ของตนในพื้นที่โซเซียลมีดีของผู้อื่นผิดกฎหมายหรือไม่</t>
-  </si>
-  <si>
     <t>การแชร์</t>
   </si>
   <si>
@@ -178,9 +169,6 @@
     <t>สาม</t>
   </si>
   <si>
-    <t>ขั้นตอนการจดทะเบียนพาณิชย์ในการค้าขายออนไลน์มีอะไรบ้าง</t>
-  </si>
-  <si>
     <t>ขั้นตอนการจดทะเบียนการค้า</t>
   </si>
   <si>
@@ -340,9 +328,6 @@
     <t>ห้า</t>
   </si>
   <si>
-    <t>ร้านขายของออนไลน์แบบไหน ที่ต้องจดทะเบียนพาณิชย์อิเล็กทรอนิกส์</t>
-  </si>
-  <si>
     <t>กฎหมายการขายของอิเล็กทรอนิกส์</t>
   </si>
   <si>
@@ -358,24 +343,9 @@
     <t>กฎหมายควบคุมการขายออนไลน์</t>
   </si>
   <si>
-    <t>ทะเบียนพาณิชย์อิเล็กทรอนิกส์</t>
-  </si>
-  <si>
-    <t>ร้านแบบไหนต้องขดทะเบียนอิเล็กทรอนิกส์</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ร้านขายของออนไลน์แบบไหน </t>
-  </si>
-  <si>
     <t>ร้านที่ต้องจดทะเบียนอิเล็กทรอนิกส์</t>
   </si>
   <si>
-    <t>จดทะเบียนพาณิชย์อิเล็กทรอนิกส์</t>
-  </si>
-  <si>
-    <t>การจดทะเบียนพาณิชย์อิเล็กทรอนิกส์</t>
-  </si>
-  <si>
     <t>การจดทะเบียนอิเล็กทรอนิกส์</t>
   </si>
   <si>
@@ -388,9 +358,6 @@
     <t>หก</t>
   </si>
   <si>
-    <t>กฎหมายขายของออนไลน์เกี่ยวข้องอย่างไรกับกฎหมายคุ้มครองผู้บริโภค</t>
-  </si>
-  <si>
     <t>กฎหมายคุ้มครองผู้บริโภค</t>
   </si>
   <si>
@@ -406,12 +373,6 @@
     <t>กฎหมายขายออนไลน์กฎหมายคุ้มครองผู้บริโภค</t>
   </si>
   <si>
-    <t>กฎหมายขายออนไลน์กับกฎหมายคุ้มครองผู้บริโภค</t>
-  </si>
-  <si>
-    <t>กฎหมายขายของออนไลน์กับกฎหมาย</t>
-  </si>
-  <si>
     <t>คุ้มครองผู้บริโภค</t>
   </si>
   <si>
@@ -692,6 +653,9 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>ทะเบียนอิเล็กทรอนิกส์</t>
   </si>
 </sst>
 </file>
@@ -1070,8 +1034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A210" workbookViewId="0">
-      <selection activeCell="B214" sqref="B214"/>
+    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="E123" sqref="E123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1084,28 +1048,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
+    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -1113,7 +1063,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -1121,7 +1071,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -1129,7 +1079,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -1137,7 +1087,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -1145,7 +1095,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -1153,7 +1103,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -1161,7 +1111,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -1169,7 +1119,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -1177,7 +1127,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -1185,7 +1135,7 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -1193,7 +1143,7 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -1201,7 +1151,7 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -1209,7 +1159,7 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -1217,7 +1167,7 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -1225,7 +1175,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -1233,1319 +1183,1274 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" t="s">
-        <v>23</v>
-      </c>
-    </row>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" t="s">
         <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B31" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B32" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B33" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B34" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B35" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B36" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B38" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B39" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B41" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B42" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B43" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B44" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B45" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B46" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B47" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B48" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B49" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>51</v>
-      </c>
-      <c r="B51" t="s">
-        <v>52</v>
-      </c>
-    </row>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
     <row r="52" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B52" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B53" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>48</v>
+      </c>
+      <c r="B54" t="s">
         <v>51</v>
-      </c>
-      <c r="B54" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B55" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B56" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B57" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B58" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B59" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B60" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B61" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B62" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B63" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B64" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B65" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B66" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B67" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B68" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B69" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B70" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B71" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B72" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B73" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B74" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B75" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B76" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B77" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B78" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B79" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B80" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B81" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B82" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B83" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>78</v>
+      </c>
+      <c r="B84" t="s">
         <v>82</v>
-      </c>
-      <c r="B84" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B85" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B86" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B87" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B88" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B89" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B90" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B91" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B92" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B93" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B94" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B95" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B96" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B97" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B98" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B99" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B100" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B101" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B102" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>105</v>
-      </c>
-      <c r="B104" t="s">
-        <v>106</v>
-      </c>
-    </row>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
     <row r="105" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B105" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B106" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B107" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
+        <v>101</v>
+      </c>
+      <c r="B108" t="s">
         <v>105</v>
-      </c>
-      <c r="B108" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B109" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B110" t="s">
-        <v>112</v>
+        <v>211</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B111" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B112" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B113" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B114" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>105</v>
-      </c>
-      <c r="B115" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>105</v>
-      </c>
-      <c r="B116" t="s">
-        <v>117</v>
-      </c>
-    </row>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="116" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
     <row r="117" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B117" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B118" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B119" t="s">
-        <v>120</v>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>111</v>
+      </c>
+      <c r="B120" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B121" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B122" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B123" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B124" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>121</v>
-      </c>
-      <c r="B125" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>121</v>
-      </c>
-      <c r="B126" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>121</v>
-      </c>
-      <c r="B127" t="s">
-        <v>128</v>
-      </c>
-    </row>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="126" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="127" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
     <row r="128" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
+        <v>120</v>
+      </c>
+      <c r="B128" t="s">
         <v>121</v>
-      </c>
-      <c r="B128" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B129" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B130" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B131" t="s">
-        <v>132</v>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>120</v>
+      </c>
+      <c r="B132" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="B133" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="B134" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="B135" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="B136" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="B137" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="B138" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="B139" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
+        <v>120</v>
+      </c>
+      <c r="B140" t="s">
         <v>133</v>
-      </c>
-      <c r="B140" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="B141" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="B142" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="B143" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="B144" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="B145" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="B146" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="B147" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="B148" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="B149" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="B150" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="B151" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="B152" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>133</v>
-      </c>
-      <c r="B153" t="s">
-        <v>153</v>
-      </c>
-    </row>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
     <row r="154" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="B154" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="B155" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="B156" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="B157" t="s">
-        <v>157</v>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>145</v>
+      </c>
+      <c r="B158" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B159" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B160" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B161" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B162" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B163" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B164" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B165" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B166" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
+        <v>145</v>
+      </c>
+      <c r="B167" t="s">
         <v>158</v>
-      </c>
-      <c r="B167" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B168" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B169" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B170" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B171" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B172" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B173" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B174" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B175" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B176" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
-        <v>158</v>
-      </c>
-      <c r="B177" t="s">
-        <v>173</v>
-      </c>
-    </row>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
     <row r="178" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="B178" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="B179" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="B180" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="B181" t="s">
-        <v>179</v>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>167</v>
+      </c>
+      <c r="B182" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="B183" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="B184" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="B185" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="B186" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="B187" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="B188" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="B189" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
-        <v>180</v>
-      </c>
-      <c r="B190" t="s">
-        <v>188</v>
-      </c>
-    </row>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
     <row r="191" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>180</v>
       </c>
       <c r="B191" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -2553,7 +2458,7 @@
         <v>180</v>
       </c>
       <c r="B192" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -2561,7 +2466,7 @@
         <v>180</v>
       </c>
       <c r="B193" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -2569,237 +2474,211 @@
         <v>180</v>
       </c>
       <c r="B194" t="s">
-        <v>192</v>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>180</v>
+      </c>
+      <c r="B195" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="B196" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="197" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A197" t="s">
-        <v>193</v>
-      </c>
-      <c r="B197" t="s">
-        <v>195</v>
-      </c>
-    </row>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
     <row r="198" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="B198" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="B199" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="B200" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="B201" t="s">
-        <v>220</v>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>208</v>
+      </c>
+      <c r="B202" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="B203" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="B204" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="B205" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="B206" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="B207" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="B208" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="B209" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="B210" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="B211" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="B212" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="B213" t="s">
-        <v>222</v>
+        <v>200</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="B214" t="s">
-        <v>223</v>
+        <v>201</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="B215" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="B216" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="B217" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="B218" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="B219" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="220" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A220" t="s">
-        <v>199</v>
-      </c>
-      <c r="B220" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="221" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A221" t="s">
-        <v>199</v>
-      </c>
-      <c r="B221" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="222" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A222" t="s">
-        <v>199</v>
-      </c>
-      <c r="B222" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="223" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A223" t="s">
-        <v>199</v>
-      </c>
-      <c r="B223" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="224" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A224" t="s">
-        <v>199</v>
-      </c>
-      <c r="B224" t="s">
-        <v>219</v>
-      </c>
-    </row>
+        <v>206</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="221" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="222" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="223" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="224" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:B200 A202:B202 A201 A215:B224 B203 B204 B205 B206 B207 B208 B209 B210 B211 B212" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:B1 A105:B109 A52:B103 A23:B50 A4:B21 A110" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add more keyword in no.4
</commit_message>
<xml_diff>
--- a/data/train.xlsx
+++ b/data/train.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project_chatbot\chat_bot_team\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53759A9D-54A0-40B8-B155-333A94101B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA166DA5-674B-4A13-8E31-E0BF5F3290B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="192">
   <si>
     <t>tag</t>
   </si>
@@ -590,6 +590,12 @@
   </si>
   <si>
     <t>ทะเบียนอิเล็กทรอนิกส์</t>
+  </si>
+  <si>
+    <t>แรก</t>
+  </si>
+  <si>
+    <t>ขั้นแรก</t>
   </si>
 </sst>
 </file>
@@ -966,15 +972,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B224"/>
+  <dimension ref="A1:B198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="G62" sqref="G62"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -982,8 +988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -991,7 +996,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -999,7 +1004,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1007,7 +1012,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1015,7 +1020,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1023,7 +1028,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1031,7 +1036,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1039,7 +1044,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1047,7 +1052,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -1055,7 +1060,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -1063,7 +1068,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -1071,9 +1076,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1081,7 +1084,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1089,7 +1092,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -1097,7 +1100,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -1105,7 +1108,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -1121,7 +1124,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -1129,7 +1132,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -1137,7 +1140,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -1145,7 +1148,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -1153,7 +1156,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -1161,7 +1164,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -1169,7 +1172,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -1177,7 +1180,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -1185,7 +1188,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -1193,7 +1196,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -1201,7 +1204,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>14</v>
       </c>
@@ -1209,7 +1212,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -1217,7 +1220,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>14</v>
       </c>
@@ -1225,7 +1228,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -1233,7 +1236,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -1241,7 +1244,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -1249,7 +1252,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>14</v>
       </c>
@@ -1257,7 +1260,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -1265,7 +1268,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -1273,7 +1276,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -1281,7 +1284,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>14</v>
       </c>
@@ -1289,9 +1292,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>42</v>
       </c>
@@ -1299,7 +1300,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>42</v>
       </c>
@@ -1307,7 +1308,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>42</v>
       </c>
@@ -1315,7 +1316,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>42</v>
       </c>
@@ -1323,7 +1324,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>42</v>
       </c>
@@ -1339,7 +1340,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>42</v>
       </c>
@@ -1347,7 +1348,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>42</v>
       </c>
@@ -1355,7 +1356,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>42</v>
       </c>
@@ -1363,7 +1364,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>42</v>
       </c>
@@ -1371,7 +1372,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>42</v>
       </c>
@@ -1379,7 +1380,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>42</v>
       </c>
@@ -1387,7 +1388,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>42</v>
       </c>
@@ -1395,7 +1396,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>42</v>
       </c>
@@ -1403,8 +1404,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>57</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>57</v>
       </c>
@@ -1420,7 +1420,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>57</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>57</v>
       </c>
@@ -1436,7 +1436,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>57</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>57</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>57</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>57</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>57</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>57</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>57</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>57</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>57</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>57</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>57</v>
       </c>
@@ -1524,7 +1524,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>57</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>57</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>57</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>57</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>57</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>57</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>57</v>
       </c>
@@ -1580,9 +1580,23 @@
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="83" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="84" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>57</v>
+      </c>
+      <c r="B82" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>57</v>
+      </c>
+      <c r="B83" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>80</v>
       </c>
@@ -1590,7 +1604,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>80</v>
       </c>
@@ -1598,7 +1612,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>80</v>
       </c>
@@ -1606,7 +1620,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>80</v>
       </c>
@@ -1614,7 +1628,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>80</v>
       </c>
@@ -1622,7 +1636,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>80</v>
       </c>
@@ -1630,7 +1644,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>80</v>
       </c>
@@ -1638,7 +1652,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>80</v>
       </c>
@@ -1646,7 +1660,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>80</v>
       </c>
@@ -1654,10 +1668,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="94" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="95" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="96" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>89</v>
       </c>
@@ -1665,7 +1676,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>89</v>
       </c>
@@ -1673,7 +1684,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>89</v>
       </c>
@@ -1681,7 +1692,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>89</v>
       </c>
@@ -1689,7 +1700,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>89</v>
       </c>
@@ -1697,7 +1708,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>89</v>
       </c>
@@ -1705,7 +1716,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>89</v>
       </c>
@@ -1721,10 +1732,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="105" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="106" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="107" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>98</v>
       </c>
@@ -1732,7 +1740,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>98</v>
       </c>
@@ -1740,7 +1748,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>98</v>
       </c>
@@ -1748,7 +1756,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>98</v>
       </c>
@@ -1756,7 +1764,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>98</v>
       </c>
@@ -1764,7 +1772,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>98</v>
       </c>
@@ -1772,7 +1780,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>98</v>
       </c>
@@ -1780,7 +1788,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>98</v>
       </c>
@@ -1788,7 +1796,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>98</v>
       </c>
@@ -1796,7 +1804,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>98</v>
       </c>
@@ -1804,7 +1812,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>98</v>
       </c>
@@ -1812,7 +1820,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>98</v>
       </c>
@@ -1820,7 +1828,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>98</v>
       </c>
@@ -1836,7 +1844,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>98</v>
       </c>
@@ -1844,7 +1852,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>98</v>
       </c>
@@ -1852,7 +1860,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>98</v>
       </c>
@@ -1860,7 +1868,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="124" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>98</v>
       </c>
@@ -1868,7 +1876,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="125" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>98</v>
       </c>
@@ -1876,7 +1884,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="126" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>98</v>
       </c>
@@ -1884,7 +1892,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="127" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>98</v>
       </c>
@@ -1892,7 +1900,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="128" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>98</v>
       </c>
@@ -1900,7 +1908,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>98</v>
       </c>
@@ -1908,7 +1916,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>98</v>
       </c>
@@ -1916,7 +1924,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="131" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>98</v>
       </c>
@@ -1924,7 +1932,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="133" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>123</v>
       </c>
@@ -1932,7 +1940,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="134" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>123</v>
       </c>
@@ -1940,7 +1948,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="135" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>123</v>
       </c>
@@ -1948,7 +1956,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="136" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>123</v>
       </c>
@@ -1956,7 +1964,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="137" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>123</v>
       </c>
@@ -1964,7 +1972,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="138" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>123</v>
       </c>
@@ -1972,7 +1980,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="139" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>123</v>
       </c>
@@ -1980,7 +1988,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="140" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>123</v>
       </c>
@@ -1988,7 +1996,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="141" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>123</v>
       </c>
@@ -1996,7 +2004,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="142" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>123</v>
       </c>
@@ -2004,7 +2012,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="143" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>123</v>
       </c>
@@ -2012,7 +2020,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="144" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>123</v>
       </c>
@@ -2020,7 +2028,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>123</v>
       </c>
@@ -2028,7 +2036,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="146" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>123</v>
       </c>
@@ -2036,7 +2044,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="147" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>123</v>
       </c>
@@ -2044,7 +2052,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="148" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>123</v>
       </c>
@@ -2052,7 +2060,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="149" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>123</v>
       </c>
@@ -2060,7 +2068,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="150" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>123</v>
       </c>
@@ -2068,7 +2076,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>123</v>
       </c>
@@ -2076,7 +2084,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>123</v>
       </c>
@@ -2084,7 +2092,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>123</v>
       </c>
@@ -2092,7 +2100,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="154" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>123</v>
       </c>
@@ -2100,7 +2108,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="155" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>123</v>
       </c>
@@ -2108,8 +2116,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="156" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="157" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>145</v>
       </c>
@@ -2125,7 +2132,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="159" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>145</v>
       </c>
@@ -2133,7 +2140,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="160" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>145</v>
       </c>
@@ -2141,7 +2148,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="161" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>145</v>
       </c>
@@ -2149,7 +2156,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="162" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>145</v>
       </c>
@@ -2157,7 +2164,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="163" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>145</v>
       </c>
@@ -2165,7 +2172,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="164" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>145</v>
       </c>
@@ -2173,7 +2180,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="165" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>145</v>
       </c>
@@ -2181,7 +2188,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="166" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>145</v>
       </c>
@@ -2189,7 +2196,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="167" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>145</v>
       </c>
@@ -2197,7 +2204,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>145</v>
       </c>
@@ -2205,8 +2212,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="169" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="170" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>158</v>
       </c>
@@ -2214,7 +2220,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="171" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>158</v>
       </c>
@@ -2222,7 +2228,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="172" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>158</v>
       </c>
@@ -2230,7 +2236,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="173" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>158</v>
       </c>
@@ -2238,7 +2244,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="174" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>158</v>
       </c>
@@ -2246,7 +2252,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="175" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>158</v>
       </c>
@@ -2254,8 +2260,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="176" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="177" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>186</v>
       </c>
@@ -2263,7 +2268,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="178" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>186</v>
       </c>
@@ -2271,7 +2276,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="179" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>186</v>
       </c>
@@ -2279,7 +2284,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="180" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>186</v>
       </c>
@@ -2287,7 +2292,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="181" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>186</v>
       </c>
@@ -2303,7 +2308,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="183" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>186</v>
       </c>
@@ -2311,7 +2316,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="184" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>186</v>
       </c>
@@ -2319,7 +2324,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="185" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>186</v>
       </c>
@@ -2327,7 +2332,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="186" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>186</v>
       </c>
@@ -2335,7 +2340,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="187" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>186</v>
       </c>
@@ -2343,7 +2348,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="188" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>186</v>
       </c>
@@ -2351,7 +2356,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>164</v>
       </c>
@@ -2359,7 +2364,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>164</v>
       </c>
@@ -2367,7 +2372,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="191" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>164</v>
       </c>
@@ -2375,7 +2380,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="192" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>164</v>
       </c>
@@ -2383,7 +2388,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="193" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>164</v>
       </c>
@@ -2391,7 +2396,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="194" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>164</v>
       </c>
@@ -2407,7 +2412,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="196" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>164</v>
       </c>
@@ -2415,7 +2420,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="197" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>164</v>
       </c>
@@ -2423,7 +2428,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>164</v>
       </c>
@@ -2431,31 +2436,6 @@
         <v>184</v>
       </c>
     </row>
-    <row r="199" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="200" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="201" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="203" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="204" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="205" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="206" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="207" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="208" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="209" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="210" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="211" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="212" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="213" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="214" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="215" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="216" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="217" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="218" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="219" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="220" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="221" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="222" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="223" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="224" ht="15" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
use last excel file
</commit_message>
<xml_diff>
--- a/data/train.xlsx
+++ b/data/train.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:B198"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -387,137 +387,1442 @@
       <c r="B1" t="str">
         <v>question</v>
       </c>
-      <c r="C1" t="str">
-        <v>full_question</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>หนึ่ง</v>
-      </c>
-      <c r="B2" t="str">
-        <v>ข้อหนึ่ง</v>
-      </c>
-      <c r="C2" t="str">
-        <v>กฎหมายที่เกี่ยวข้องกับการขายของออนไลน์มีกฎหมายสำคัญๆใดที่เกี่ยวข้องบ้าง</v>
-      </c>
-      <c r="D2" t="str">
-        <v/>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>สอง</v>
+        <v>หนึ่ง</v>
       </c>
       <c r="B3" t="str">
-        <v>ข้อสอง</v>
-      </c>
-      <c r="C3" t="str">
-        <v>การแชร์รูปภาพหรือข้อความต่างๆ เกี่ยวกับร้านค้าออนไลน์ของตนในพื้นที่โซเซียลมีดีของผู้อื่นผิดกฎหมายหรือไม่</v>
+        <v>กฎหมายสำคัญ</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>สาม</v>
+        <v>หนึ่ง</v>
       </c>
       <c r="B4" t="str">
-        <v>ข้อสาม</v>
-      </c>
-      <c r="C4" t="str">
-        <v>ขั้นตอนการจดทะเบียนพาณิชย์ในการค้าขายออนไลน์มีอะไรบ้าง</v>
+        <v>กฎหมายควรรู้</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>สี่</v>
+        <v>หนึ่ง</v>
       </c>
       <c r="B5" t="str">
-        <v>ข้อสี่</v>
-      </c>
-      <c r="C5" t="str">
-        <v>ขั้นตอนแรกก่อนขายของออนไลน์ต้องทำอย่างไรบ้าง</v>
+        <v>กฎหมายที่ควรรู้</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>ห้า</v>
+        <v>หนึ่ง</v>
       </c>
       <c r="B6" t="str">
-        <v>ข้อห้า</v>
-      </c>
-      <c r="C6" t="str">
-        <v>กฎหมายเกี่ยวกับการขายของออนไลน์มีไว้ทำไม</v>
+        <v>กฎหมายขายของออนไลน์ที่ต้องรู้</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>หก</v>
+        <v>หนึ่ง</v>
       </c>
       <c r="B7" t="str">
-        <v>ข้อหก</v>
-      </c>
-      <c r="C7" t="str">
-        <v>กฎหมายขายของออนไลน์เกี่ยวข้องอย่างไรกับกฎหมายคุ้มครองผู้บริโภค</v>
+        <v>กฎหมายขายของออนไลน์สำคัญๆ</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>เจ็ด</v>
+        <v>หนึ่ง</v>
       </c>
       <c r="B8" t="str">
-        <v>ข้อเจ็ด</v>
-      </c>
-      <c r="C8" t="str">
-        <v>สินค้าที่ห้ามขายออนไลน์มีอะไรบ้าง</v>
+        <v>กฎหมายขายของออนไลน์ที่เกี่ยวข้อง</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>แปด</v>
+        <v>หนึ่ง</v>
       </c>
       <c r="B9" t="str">
-        <v>ข้อแปด</v>
-      </c>
-      <c r="C9" t="str">
-        <v>ร้านค้าออนไลน์ควรแสดงรายละเอียดอะไรบ้าง</v>
+        <v>เกี่ยวข้องกับการขายของออนไลน์</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>เก้า</v>
+        <v>หนึ่ง</v>
       </c>
       <c r="B10" t="str">
-        <v>ข้อเก้า</v>
-      </c>
-      <c r="C10" t="str">
-        <v>ร้านค้าออนไลน์ต้องเสียภาษีอย่างไร</v>
+        <v>เกี่ยวข้องกับการขายออนไลน์</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>สิบ</v>
+        <v>หนึ่ง</v>
       </c>
       <c r="B11" t="str">
-        <v>ข้อสิบ</v>
-      </c>
-      <c r="C11" t="str">
-        <v>ร้านค้าออนไลน์จะขายตรงและตลาดแบบตรงได้หรือไม่</v>
+        <v>เกี่ยวข้องกับ</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
+        <v>หนึ่ง</v>
+      </c>
+      <c r="B12" t="str">
+        <v>กฎหมายสำคัญๆ</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>หนึ่ง</v>
+      </c>
+      <c r="B13" t="str">
+        <v>สำคัญ</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>สอง</v>
+      </c>
+      <c r="B16" t="str">
+        <v>การแชร์</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>สอง</v>
+      </c>
+      <c r="B17" t="str">
+        <v>แชร์ภาพ</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>สอง</v>
+      </c>
+      <c r="B18" t="str">
+        <v>แชร์ข้อความ</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>สอง</v>
+      </c>
+      <c r="B19" t="str">
+        <v>แชร์โพสต์</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>สอง</v>
+      </c>
+      <c r="B20" t="str">
+        <v>การแชร์โพสต์</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>สอง</v>
+      </c>
+      <c r="B21" t="str">
+        <v>การแชร์ภาพ</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>สอง</v>
+      </c>
+      <c r="B22" t="str">
+        <v>แชร์โพส</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>สอง</v>
+      </c>
+      <c r="B23" t="str">
+        <v>การแชร์ภาพในที่</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>สอง</v>
+      </c>
+      <c r="B24" t="str">
+        <v>การแชร์ภาพในกลุ่ม</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>สอง</v>
+      </c>
+      <c r="B25" t="str">
+        <v>การแชร์ภาพในที่สาธารณะ</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>สอง</v>
+      </c>
+      <c r="B26" t="str">
+        <v>การแชร์ภาพในที่คนอื่น</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>สอง</v>
+      </c>
+      <c r="B27" t="str">
+        <v>การแชร์โพสในที่สาธารณะ</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>สอง</v>
+      </c>
+      <c r="B28" t="str">
+        <v>การแชร์โพสในกลุ่ม</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>สอง</v>
+      </c>
+      <c r="B29" t="str">
+        <v>การแชร์โพสต์ในที่</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>สอง</v>
+      </c>
+      <c r="B30" t="str">
+        <v>การแชร์ข้อความในที่</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>สอง</v>
+      </c>
+      <c r="B31" t="str">
+        <v>การแชร์ข้อความในที่สาธารณะ</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>สอง</v>
+      </c>
+      <c r="B32" t="str">
+        <v>การแชร์ข้อความในที่คนอื่น</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>สอง</v>
+      </c>
+      <c r="B33" t="str">
+        <v>การแชร์ต่างๆ</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>สอง</v>
+      </c>
+      <c r="B34" t="str">
+        <v>กฎหมายการแชร์</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>สอง</v>
+      </c>
+      <c r="B35" t="str">
+        <v>กฎหมายแชร์</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>สอง</v>
+      </c>
+      <c r="B36" t="str">
+        <v>กฎหมายโปรโมท</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>สอง</v>
+      </c>
+      <c r="B37" t="str">
+        <v>กฎหมายแนะนำร้าน</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>สอง</v>
+      </c>
+      <c r="B38" t="str">
+        <v>กฎหมายแชร์ร้าน</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>สอง</v>
+      </c>
+      <c r="B39" t="str">
+        <v>กฎหมายฝากร้าน</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>สอง</v>
+      </c>
+      <c r="B40" t="str">
+        <v>การฝากร้าน</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>สอง</v>
+      </c>
+      <c r="B41" t="str">
+        <v>ฝากร้าน</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>สอง</v>
+      </c>
+      <c r="B42" t="str">
+        <v>ฝากร้านได้</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>สาม</v>
+      </c>
+      <c r="B45" t="str">
+        <v>ขั้นตอนการจดทะเบียนการค้า</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>สาม</v>
+      </c>
+      <c r="B46" t="str">
+        <v>ขั้นตอนการจดทะเบียน</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>สาม</v>
+      </c>
+      <c r="B47" t="str">
+        <v>ขั้นตอนการจดทะเบียนร้านค้า</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>สาม</v>
+      </c>
+      <c r="B48" t="str">
+        <v>ขั้นตอนการจดทะเบียนออนไลน์</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>สาม</v>
+      </c>
+      <c r="B49" t="str">
+        <v>ขั้นตอนการจดทะเบียนพาณิชย์</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>สาม</v>
+      </c>
+      <c r="B50" t="str">
+        <v>ขั้นตอนการจดทะเบียนพาณิชย์ร้านค้า</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>สาม</v>
+      </c>
+      <c r="B51" t="str">
+        <v>ขั้นตอนการจดทะเบียนร้านค้าออนไลน์</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>สาม</v>
+      </c>
+      <c r="B52" t="str">
+        <v>ขั้นตอนการจด</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>สาม</v>
+      </c>
+      <c r="B53" t="str">
+        <v>ขั้นตอนทะเบียนการค้า</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>สาม</v>
+      </c>
+      <c r="B54" t="str">
+        <v>ขั้นตอนทะเบียน</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>สาม</v>
+      </c>
+      <c r="B55" t="str">
+        <v>ขั้นตอนทะเบียนพาณิชย์</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>สาม</v>
+      </c>
+      <c r="B56" t="str">
+        <v>ขั้นตอนพาณิชย์</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>สาม</v>
+      </c>
+      <c r="B57" t="str">
+        <v>ขั้นตอนจดทะเบียน</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>สาม</v>
+      </c>
+      <c r="B58" t="str">
+        <v>ขั้นตอน</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>สี่</v>
+      </c>
+      <c r="B60" t="str">
+        <v>การเปิดร้าน</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>สี่</v>
+      </c>
+      <c r="B61" t="str">
+        <v>ขั้นตอนแรกก่อนขายของออนไลน์ต้องทำอย่างไร</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>สี่</v>
+      </c>
+      <c r="B62" t="str">
+        <v>ก่อนขายของออนไลน์</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>สี่</v>
+      </c>
+      <c r="B63" t="str">
+        <v>ก่อนขายออนไลน์</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>สี่</v>
+      </c>
+      <c r="B64" t="str">
+        <v>ก่อนการค้าขายออนไลน์</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>สี่</v>
+      </c>
+      <c r="B65" t="str">
+        <v>ก่อนการซื้อขายออนไลน์</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>สี่</v>
+      </c>
+      <c r="B66" t="str">
+        <v>ก่อนการเปิดร้านออนไลน์</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>สี่</v>
+      </c>
+      <c r="B67" t="str">
+        <v>ก่อนการเริ่มต้น</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>สี่</v>
+      </c>
+      <c r="B68" t="str">
+        <v>ก่อนการเปิดตัว</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>สี่</v>
+      </c>
+      <c r="B69" t="str">
+        <v>ก่อนการเริ่มสร้าง</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>สี่</v>
+      </c>
+      <c r="B70" t="str">
+        <v>ก่อนการเปิดร้าน</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>สี่</v>
+      </c>
+      <c r="B71" t="str">
+        <v>ก่อนการเริ่มธุรกิจ</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>สี่</v>
+      </c>
+      <c r="B72" t="str">
+        <v>เริ่มต้น</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>สี่</v>
+      </c>
+      <c r="B73" t="str">
+        <v>เริ่มต้นสร้าง</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>สี่</v>
+      </c>
+      <c r="B74" t="str">
+        <v>เริ่มต้นเปิด</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>สี่</v>
+      </c>
+      <c r="B75" t="str">
+        <v>เริ่มต้นการ</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>สี่</v>
+      </c>
+      <c r="B76" t="str">
+        <v>เริ่มต้นซื้อของ</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>สี่</v>
+      </c>
+      <c r="B77" t="str">
+        <v>เริ่มต้นซื้อขาย</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>สี่</v>
+      </c>
+      <c r="B78" t="str">
+        <v>เริ่มต้นเปิดร้าน</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>สี่</v>
+      </c>
+      <c r="B79" t="str">
+        <v>เริ่มต้นขายของ</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>สี่</v>
+      </c>
+      <c r="B80" t="str">
+        <v>เริ่มต้นขายของออนไลน์</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>สี่</v>
+      </c>
+      <c r="B81" t="str">
+        <v>เริ่มต้นขายออนไลน์</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>ห้า</v>
+      </c>
+      <c r="B84" t="str">
+        <v>กฎหมายการขายของอิเล็กทรอนิกส์</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>ห้า</v>
+      </c>
+      <c r="B85" t="str">
+        <v>กฎหมายขายของอิเล็กทรอนิกส์</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>ห้า</v>
+      </c>
+      <c r="B86" t="str">
+        <v>จดทะเบียนอิเล็กทรอนิกส์</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>ห้า</v>
+      </c>
+      <c r="B87" t="str">
+        <v>อิเล็กทรอนิกส์</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>ห้า</v>
+      </c>
+      <c r="B88" t="str">
+        <v>ทะเบียนอิเล็กทรอนิกส์</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>ห้า</v>
+      </c>
+      <c r="B89" t="str">
+        <v>ร้านที่ต้องจดทะเบียนอิเล็กทรอนิกส์</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>ห้า</v>
+      </c>
+      <c r="B90" t="str">
+        <v>การจดทะเบียนอิเล็กทรอนิกส์</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="str">
+        <v>ห้า</v>
+      </c>
+      <c r="B91" t="str">
+        <v>DBD Registered</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v>ห้า</v>
+      </c>
+      <c r="B92" t="str">
+        <v>dbd registered</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="str">
+        <v>หก</v>
+      </c>
+      <c r="B96" t="str">
+        <v>กฎหมายคุ้มครองผู้บริโภค</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="str">
+        <v>หก</v>
+      </c>
+      <c r="B97" t="str">
+        <v>กฎหมายคุ้มครอง</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="str">
+        <v>หก</v>
+      </c>
+      <c r="B98" t="str">
+        <v>กฎหมายผู้บริโภค</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="str">
+        <v>หก</v>
+      </c>
+      <c r="B99" t="str">
+        <v>กฎหมายขายของออนไลน์กับกฎหมายคุ้มครองผู้บริโภค</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="str">
+        <v>หก</v>
+      </c>
+      <c r="B100" t="str">
+        <v>กฎหมายขายออนไลน์กฎหมายคุ้มครองผู้บริโภค</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="str">
+        <v>หก</v>
+      </c>
+      <c r="B101" t="str">
+        <v>คุ้มครองผู้บริโภค</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="str">
+        <v>หก</v>
+      </c>
+      <c r="B102" t="str">
+        <v>คุ้มครอง</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="str">
+        <v>หก</v>
+      </c>
+      <c r="B103" t="str">
+        <v>ผู้บริโภค</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="str">
+        <v>เจ็ด</v>
+      </c>
+      <c r="B107" t="str">
+        <v>สินค้าที่ห้ามขายออนไลน์</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="str">
+        <v>เจ็ด</v>
+      </c>
+      <c r="B108" t="str">
+        <v>สินค้าห้ามขาย</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="str">
+        <v>เจ็ด</v>
+      </c>
+      <c r="B109" t="str">
+        <v>สินค้าต้องห้าม</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="str">
+        <v>เจ็ด</v>
+      </c>
+      <c r="B110" t="str">
+        <v>สินค้าผิดกฎหมาย</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="str">
+        <v>เจ็ด</v>
+      </c>
+      <c r="B111" t="str">
+        <v>สินค้าผิด</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="str">
+        <v>เจ็ด</v>
+      </c>
+      <c r="B112" t="str">
+        <v>สินค้าลักลอบ</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="str">
+        <v>เจ็ด</v>
+      </c>
+      <c r="B113" t="str">
+        <v>สินค้าไม่ดี</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="str">
+        <v>เจ็ด</v>
+      </c>
+      <c r="B114" t="str">
+        <v>สินค้าห้าม</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="str">
+        <v>เจ็ด</v>
+      </c>
+      <c r="B115" t="str">
+        <v>สินค้าอันตราย</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="str">
+        <v>เจ็ด</v>
+      </c>
+      <c r="B116" t="str">
+        <v>สินค้าที่ห้าม</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="str">
+        <v>เจ็ด</v>
+      </c>
+      <c r="B117" t="str">
+        <v>สินค้าที่ห้ามขายของออนไลน์</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="str">
+        <v>เจ็ด</v>
+      </c>
+      <c r="B118" t="str">
+        <v>สินค้าที่ห้ามขายบนออนไลน์</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="str">
+        <v>เจ็ด</v>
+      </c>
+      <c r="B119" t="str">
+        <v>สินค้าที่ผิดกฎหมาย</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="str">
+        <v>เจ็ด</v>
+      </c>
+      <c r="B120" t="str">
+        <v>สินค้าที่ห้าม</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="str">
+        <v>เจ็ด</v>
+      </c>
+      <c r="B121" t="str">
+        <v>สินค้าที่ห้ามนำมาขาย</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="str">
+        <v>เจ็ด</v>
+      </c>
+      <c r="B122" t="str">
+        <v>สินค้าที่ห้ามจำหน่าย</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="str">
+        <v>เจ็ด</v>
+      </c>
+      <c r="B123" t="str">
+        <v>สินค้าที่ห้ามจำหน่ายออนไลน์</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="str">
+        <v>เจ็ด</v>
+      </c>
+      <c r="B124" t="str">
+        <v>สินค้าที่ห้ามจำหน่ายผิดกฎหมาย</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="str">
+        <v>เจ็ด</v>
+      </c>
+      <c r="B125" t="str">
+        <v>ห้ามขาย</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="str">
+        <v>เจ็ด</v>
+      </c>
+      <c r="B126" t="str">
+        <v>ห้ามจำหน่าย</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="str">
+        <v>เจ็ด</v>
+      </c>
+      <c r="B127" t="str">
+        <v>ห้ามขายออนไลน์</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="str">
+        <v>เจ็ด</v>
+      </c>
+      <c r="B128" t="str">
+        <v>ห้ามขายของออนไลน์</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="str">
+        <v>เจ็ด</v>
+      </c>
+      <c r="B129" t="str">
+        <v>ห้ามจำหน่ายออนไลน์</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="str">
+        <v>เจ็ด</v>
+      </c>
+      <c r="B130" t="str">
+        <v>ห้ามจำหน่ายขายของ</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="str">
+        <v>เจ็ด</v>
+      </c>
+      <c r="B131" t="str">
+        <v>ห้ามจำหน่ายขายของทางออนไลน์</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="str">
+        <v>แปด</v>
+      </c>
+      <c r="B133" t="str">
+        <v>ร้านค้าออนไลน์ควรแสดงรายละเอียด</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="str">
+        <v>แปด</v>
+      </c>
+      <c r="B134" t="str">
+        <v>แสดงรายละเอียด</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="str">
+        <v>แปด</v>
+      </c>
+      <c r="B135" t="str">
+        <v>แสดงข้อมูล</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="str">
+        <v>แปด</v>
+      </c>
+      <c r="B136" t="str">
+        <v>แสดงประวัติ</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="str">
+        <v>แปด</v>
+      </c>
+      <c r="B137" t="str">
+        <v>แสดงสินค้า</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="str">
+        <v>แปด</v>
+      </c>
+      <c r="B138" t="str">
+        <v>แสดงถึง</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="str">
+        <v>แปด</v>
+      </c>
+      <c r="B139" t="str">
+        <v>การแสดง</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="str">
+        <v>แปด</v>
+      </c>
+      <c r="B140" t="str">
+        <v>การแสดงรายละเอียด</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="str">
+        <v>แปด</v>
+      </c>
+      <c r="B141" t="str">
+        <v>การแสดงข้อมูล</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="str">
+        <v>แปด</v>
+      </c>
+      <c r="B142" t="str">
+        <v>การแสดง</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="str">
+        <v>แปด</v>
+      </c>
+      <c r="B143" t="str">
+        <v>ร้านค้าออนไลน์แสดงรายละเอียด</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="str">
+        <v>แปด</v>
+      </c>
+      <c r="B144" t="str">
+        <v>ร้านค้าออนไลน์แสดงข้อมูล</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="str">
+        <v>แปด</v>
+      </c>
+      <c r="B145" t="str">
+        <v>ร้านค้าออนไลน์แสดงประวัติ</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="str">
+        <v>แปด</v>
+      </c>
+      <c r="B146" t="str">
+        <v>ร้านค้าออนไลน์แสดงสินค้า</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="str">
+        <v>แปด</v>
+      </c>
+      <c r="B147" t="str">
+        <v>ร้านค้าออนไลน์แสดงถึง</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="str">
+        <v>แปด</v>
+      </c>
+      <c r="B148" t="str">
+        <v>ร้านค้าออนไลน์การแสดง</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="str">
+        <v>แปด</v>
+      </c>
+      <c r="B149" t="str">
+        <v>ร้านค้าออนไลน์การแสดงรายละเอียด</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="str">
+        <v>แปด</v>
+      </c>
+      <c r="B150" t="str">
+        <v>ร้านค้าออนไลน์การแสดงข้อมูล</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="str">
+        <v>แปด</v>
+      </c>
+      <c r="B151" t="str">
+        <v>ร้านค้าออนไลน์การแสดง</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="str">
+        <v>แปด</v>
+      </c>
+      <c r="B152" t="str">
+        <v>ข้อมูล</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="str">
+        <v>แปด</v>
+      </c>
+      <c r="B153" t="str">
+        <v>รายละเอียด</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="str">
+        <v>แปด</v>
+      </c>
+      <c r="B154" t="str">
+        <v>ข้อมูลร้าน</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="str">
+        <v>แปด</v>
+      </c>
+      <c r="B155" t="str">
+        <v>รายละเอียดร้าน</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="str">
+        <v>เก้า</v>
+      </c>
+      <c r="B157" t="str">
+        <v>ร้านค้าออนไลน์ต้องเสียภาษีอย่างไร</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="str">
+        <v>เก้า</v>
+      </c>
+      <c r="B158" t="str">
+        <v>เสียภาษีอย่างไร</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="str">
+        <v>เก้า</v>
+      </c>
+      <c r="B159" t="str">
+        <v>เสียภาษี</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="str">
+        <v>เก้า</v>
+      </c>
+      <c r="B160" t="str">
+        <v>ต้องเสียภาษี</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="str">
+        <v>เก้า</v>
+      </c>
+      <c r="B161" t="str">
+        <v>ต้องเสียภาษีอย่างไร</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="str">
+        <v>เก้า</v>
+      </c>
+      <c r="B162" t="str">
+        <v>ภาษี</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="str">
+        <v>เก้า</v>
+      </c>
+      <c r="B163" t="str">
+        <v>เก็บภาษี</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="str">
+        <v>เก้า</v>
+      </c>
+      <c r="B164" t="str">
+        <v>โดนเก็บภาษี</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="str">
+        <v>เก้า</v>
+      </c>
+      <c r="B165" t="str">
+        <v>ร้านค้าออนไลน์ต้องจ่ายภาษีอย่างไร</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="str">
+        <v>เก้า</v>
+      </c>
+      <c r="B166" t="str">
+        <v>จ่ายภาษีอย่างไร</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="str">
+        <v>เก้า</v>
+      </c>
+      <c r="B167" t="str">
+        <v>ต้องจ่ายภาษี</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="str">
+        <v>เก้า</v>
+      </c>
+      <c r="B168" t="str">
+        <v>จ่ายภาษี</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="str">
+        <v>สิบ</v>
+      </c>
+      <c r="B170" t="str">
+        <v>ร้านค้าออนไลน์จะขายตรงและตลาดแบบตรงได้หรือไม่</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="str">
+        <v>สิบ</v>
+      </c>
+      <c r="B171" t="str">
+        <v>ขายตรงและตลาดแบบตรง</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="str">
+        <v>สิบ</v>
+      </c>
+      <c r="B172" t="str">
+        <v>ขายตรงตลาดแบบตรง</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="str">
+        <v>สิบ</v>
+      </c>
+      <c r="B173" t="str">
+        <v>ขายตรง</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="str">
+        <v>สิบ</v>
+      </c>
+      <c r="B174" t="str">
+        <v>ตลาดแบบตรง</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="str">
+        <v>สิบ</v>
+      </c>
+      <c r="B175" t="str">
+        <v>แบบตรง</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="str">
+        <v>greet</v>
+      </c>
+      <c r="B177" t="str">
+        <v>Hello</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="str">
+        <v>greet</v>
+      </c>
+      <c r="B178" t="str">
+        <v>Hi</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="str">
+        <v>greet</v>
+      </c>
+      <c r="B179" t="str">
+        <v>Hey</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="str">
+        <v>greet</v>
+      </c>
+      <c r="B180" t="str">
+        <v>Yo</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="str">
+        <v>greet</v>
+      </c>
+      <c r="B181" t="str">
+        <v>Yep</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="str">
+        <v>greet</v>
+      </c>
+      <c r="B182" t="str">
+        <v>Sup</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="str">
+        <v>greet</v>
+      </c>
+      <c r="B183" t="str">
+        <v>What</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="str">
+        <v>greet</v>
+      </c>
+      <c r="B184" t="str">
+        <v>What's up</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="str">
+        <v>greet</v>
+      </c>
+      <c r="B185" t="str">
+        <v>Yea</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="str">
+        <v>greet</v>
+      </c>
+      <c r="B186" t="str">
+        <v>Yeah</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="str">
+        <v>greet</v>
+      </c>
+      <c r="B187" t="str">
+        <v>Yess</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="str">
+        <v>greet</v>
+      </c>
+      <c r="B188" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="str">
         <v>ทักทาย</v>
       </c>
-      <c r="B12" t="str">
+      <c r="B189" t="str">
+        <v>สวัสดี</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="str">
         <v>ทักทาย</v>
       </c>
-      <c r="C12" t="str">
+      <c r="B190" t="str">
+        <v>หวัดดี</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="str">
         <v>ทักทาย</v>
+      </c>
+      <c r="B191" t="str">
+        <v>ดีจ้า</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="str">
+        <v>ทักทาย</v>
+      </c>
+      <c r="B192" t="str">
+        <v>ดีครับ</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="str">
+        <v>ทักทาย</v>
+      </c>
+      <c r="B193" t="str">
+        <v>ดีค้าบบ</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="str">
+        <v>ทักทาย</v>
+      </c>
+      <c r="B194" t="str">
+        <v>ดีค่ะ</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="str">
+        <v>ทักทาย</v>
+      </c>
+      <c r="B195" t="str">
+        <v>สวัสดีค่ะ</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="str">
+        <v>ทักทาย</v>
+      </c>
+      <c r="B196" t="str">
+        <v>สวัสดีค้า</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="str">
+        <v>ทักทาย</v>
+      </c>
+      <c r="B197" t="str">
+        <v>สวัสดีนะ</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="str">
+        <v>ทักทาย</v>
+      </c>
+      <c r="B198" t="str">
+        <v>สวัสดีนาย</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D12"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B198"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add more keywords and more features in no 5
</commit_message>
<xml_diff>
--- a/data/train.xlsx
+++ b/data/train.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project_chatbot\chat_bot_team\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA166DA5-674B-4A13-8E31-E0BF5F3290B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06F8B5F-B381-46E2-9E00-996169DC170C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="197">
   <si>
     <t>tag</t>
   </si>
@@ -596,6 +596,21 @@
   </si>
   <si>
     <t>ขั้นแรก</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ห้า </t>
+  </si>
+  <si>
+    <t>ลักษณะร้านที่ต้องจดทะเบียนอิเล็กทรอนิกซ์</t>
+  </si>
+  <si>
+    <t>ร้านประเภทไหนต้องจดทะเบียนอิเล็กทรอนิกซ์</t>
+  </si>
+  <si>
+    <t>เปิดร้านใน shopee ต้องมีทะเบียนอิเล็กทรอนิกส์ไหม</t>
+  </si>
+  <si>
+    <t>เปิดร้านใน lazada ต้องมีทะเบียนอิเล็กทรอนิกส์ไหม</t>
   </si>
 </sst>
 </file>
@@ -974,8 +989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1668,28 +1683,44 @@
         <v>88</v>
       </c>
     </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>80</v>
+      </c>
+      <c r="B93" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>192</v>
+      </c>
+      <c r="B94" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>80</v>
+      </c>
+      <c r="B95" t="s">
+        <v>194</v>
+      </c>
+    </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B96" t="s">
-        <v>90</v>
+        <v>195</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B97" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>89</v>
-      </c>
-      <c r="B98" t="s">
-        <v>92</v>
+        <v>196</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -1697,7 +1728,7 @@
         <v>89</v>
       </c>
       <c r="B99" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -1705,7 +1736,7 @@
         <v>89</v>
       </c>
       <c r="B100" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -1713,7 +1744,7 @@
         <v>89</v>
       </c>
       <c r="B101" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
@@ -1721,7 +1752,7 @@
         <v>89</v>
       </c>
       <c r="B102" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -1729,6 +1760,30 @@
         <v>89</v>
       </c>
       <c r="B103" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>89</v>
+      </c>
+      <c r="B104" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>89</v>
+      </c>
+      <c r="B105" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>89</v>
+      </c>
+      <c r="B106" t="s">
         <v>97</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add more keywords in no 4
</commit_message>
<xml_diff>
--- a/data/train.xlsx
+++ b/data/train.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project_chatbot\chat_bot_team\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06F8B5F-B381-46E2-9E00-996169DC170C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CEE85F-9750-4919-B793-927729D7DD9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="198">
   <si>
     <t>tag</t>
   </si>
@@ -611,6 +611,9 @@
   </si>
   <si>
     <t>เปิดร้านใน lazada ต้องมีทะเบียนอิเล็กทรอนิกส์ไหม</t>
+  </si>
+  <si>
+    <t>อยากขายของออนไลน์</t>
   </si>
 </sst>
 </file>
@@ -989,8 +992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1419,6 +1422,14 @@
         <v>56</v>
       </c>
     </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>57</v>
+      </c>
+      <c r="B59" t="s">
+        <v>197</v>
+      </c>
+    </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>57</v>

</xml_diff>

<commit_message>
add more key word in no 6
</commit_message>
<xml_diff>
--- a/data/train.xlsx
+++ b/data/train.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project_chatbot\chat_bot_team\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CEE85F-9750-4919-B793-927729D7DD9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFC9CA6-BAAC-4E53-939E-FC6B46AAFBBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="200">
   <si>
     <t>tag</t>
   </si>
@@ -614,6 +614,12 @@
   </si>
   <si>
     <t>อยากขายของออนไลน์</t>
+  </si>
+  <si>
+    <t>กฎหมายลูกค้า</t>
+  </si>
+  <si>
+    <t>กฎหมายเกี่ยวกับลูกค้า</t>
   </si>
 </sst>
 </file>
@@ -990,10 +996,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B198"/>
+  <dimension ref="A1:B204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="B108" sqref="B108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1800,50 +1806,18 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B107" t="s">
-        <v>99</v>
+        <v>198</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B108" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>98</v>
-      </c>
-      <c r="B109" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>98</v>
-      </c>
-      <c r="B110" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>98</v>
-      </c>
-      <c r="B111" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>98</v>
-      </c>
-      <c r="B112" t="s">
-        <v>104</v>
+        <v>199</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
@@ -1851,7 +1825,7 @@
         <v>98</v>
       </c>
       <c r="B113" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
@@ -1859,7 +1833,7 @@
         <v>98</v>
       </c>
       <c r="B114" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -1867,7 +1841,7 @@
         <v>98</v>
       </c>
       <c r="B115" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
@@ -1875,7 +1849,7 @@
         <v>98</v>
       </c>
       <c r="B116" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
@@ -1883,7 +1857,7 @@
         <v>98</v>
       </c>
       <c r="B117" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
@@ -1891,7 +1865,7 @@
         <v>98</v>
       </c>
       <c r="B118" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
@@ -1899,7 +1873,7 @@
         <v>98</v>
       </c>
       <c r="B119" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
@@ -1907,7 +1881,7 @@
         <v>98</v>
       </c>
       <c r="B120" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
@@ -1915,7 +1889,7 @@
         <v>98</v>
       </c>
       <c r="B121" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
@@ -1923,7 +1897,7 @@
         <v>98</v>
       </c>
       <c r="B122" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
@@ -1931,7 +1905,7 @@
         <v>98</v>
       </c>
       <c r="B123" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -1939,7 +1913,7 @@
         <v>98</v>
       </c>
       <c r="B124" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
@@ -1947,7 +1921,7 @@
         <v>98</v>
       </c>
       <c r="B125" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
@@ -1955,7 +1929,7 @@
         <v>98</v>
       </c>
       <c r="B126" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
@@ -1963,7 +1937,7 @@
         <v>98</v>
       </c>
       <c r="B127" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
@@ -1971,7 +1945,7 @@
         <v>98</v>
       </c>
       <c r="B128" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
@@ -1979,7 +1953,7 @@
         <v>98</v>
       </c>
       <c r="B129" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
@@ -1987,7 +1961,7 @@
         <v>98</v>
       </c>
       <c r="B130" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
@@ -1995,55 +1969,55 @@
         <v>98</v>
       </c>
       <c r="B131" t="s">
-        <v>122</v>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>98</v>
+      </c>
+      <c r="B132" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="B133" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="B134" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="B135" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="B136" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="B137" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>123</v>
-      </c>
-      <c r="B138" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
@@ -2051,7 +2025,7 @@
         <v>123</v>
       </c>
       <c r="B139" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
@@ -2059,7 +2033,7 @@
         <v>123</v>
       </c>
       <c r="B140" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
@@ -2067,7 +2041,7 @@
         <v>123</v>
       </c>
       <c r="B141" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
@@ -2075,7 +2049,7 @@
         <v>123</v>
       </c>
       <c r="B142" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
@@ -2083,7 +2057,7 @@
         <v>123</v>
       </c>
       <c r="B143" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
@@ -2091,7 +2065,7 @@
         <v>123</v>
       </c>
       <c r="B144" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
@@ -2099,7 +2073,7 @@
         <v>123</v>
       </c>
       <c r="B145" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
@@ -2107,7 +2081,7 @@
         <v>123</v>
       </c>
       <c r="B146" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
@@ -2115,7 +2089,7 @@
         <v>123</v>
       </c>
       <c r="B147" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
@@ -2123,7 +2097,7 @@
         <v>123</v>
       </c>
       <c r="B148" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
@@ -2131,7 +2105,7 @@
         <v>123</v>
       </c>
       <c r="B149" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
@@ -2139,7 +2113,7 @@
         <v>123</v>
       </c>
       <c r="B150" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
@@ -2147,7 +2121,7 @@
         <v>123</v>
       </c>
       <c r="B151" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
@@ -2155,7 +2129,7 @@
         <v>123</v>
       </c>
       <c r="B152" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
@@ -2163,7 +2137,7 @@
         <v>123</v>
       </c>
       <c r="B153" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
@@ -2171,7 +2145,7 @@
         <v>123</v>
       </c>
       <c r="B154" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
@@ -2179,55 +2153,55 @@
         <v>123</v>
       </c>
       <c r="B155" t="s">
-        <v>144</v>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>123</v>
+      </c>
+      <c r="B156" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="B157" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="B158" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="B159" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="B160" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="B161" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
-        <v>145</v>
-      </c>
-      <c r="B162" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
@@ -2235,7 +2209,7 @@
         <v>145</v>
       </c>
       <c r="B163" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
@@ -2243,7 +2217,7 @@
         <v>145</v>
       </c>
       <c r="B164" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
@@ -2251,7 +2225,7 @@
         <v>145</v>
       </c>
       <c r="B165" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
@@ -2259,7 +2233,7 @@
         <v>145</v>
       </c>
       <c r="B166" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
@@ -2267,7 +2241,7 @@
         <v>145</v>
       </c>
       <c r="B167" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
@@ -2275,103 +2249,103 @@
         <v>145</v>
       </c>
       <c r="B168" t="s">
-        <v>157</v>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>145</v>
+      </c>
+      <c r="B169" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B170" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B171" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B172" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B173" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
+        <v>145</v>
+      </c>
+      <c r="B174" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
         <v>158</v>
       </c>
-      <c r="B174" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
-        <v>158</v>
-      </c>
-      <c r="B175" t="s">
-        <v>185</v>
+      <c r="B176" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>186</v>
+        <v>158</v>
       </c>
       <c r="B177" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>186</v>
+        <v>158</v>
       </c>
       <c r="B178" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>186</v>
+        <v>158</v>
       </c>
       <c r="B179" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>186</v>
+        <v>158</v>
       </c>
       <c r="B180" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>186</v>
+        <v>158</v>
       </c>
       <c r="B181" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
-        <v>186</v>
-      </c>
-      <c r="B182" t="s">
-        <v>170</v>
+        <v>185</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
@@ -2379,7 +2353,7 @@
         <v>186</v>
       </c>
       <c r="B183" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
@@ -2387,7 +2361,7 @@
         <v>186</v>
       </c>
       <c r="B184" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
@@ -2395,7 +2369,7 @@
         <v>186</v>
       </c>
       <c r="B185" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
@@ -2403,7 +2377,7 @@
         <v>186</v>
       </c>
       <c r="B186" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
@@ -2411,7 +2385,7 @@
         <v>186</v>
       </c>
       <c r="B187" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
@@ -2419,55 +2393,55 @@
         <v>186</v>
       </c>
       <c r="B188" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>164</v>
+        <v>186</v>
       </c>
       <c r="B189" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>164</v>
+        <v>186</v>
       </c>
       <c r="B190" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>164</v>
+        <v>186</v>
       </c>
       <c r="B191" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>164</v>
+        <v>186</v>
       </c>
       <c r="B192" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>164</v>
+        <v>186</v>
       </c>
       <c r="B193" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>164</v>
+        <v>186</v>
       </c>
       <c r="B194" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
@@ -2475,7 +2449,7 @@
         <v>164</v>
       </c>
       <c r="B195" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
@@ -2483,7 +2457,7 @@
         <v>164</v>
       </c>
       <c r="B196" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
@@ -2491,7 +2465,7 @@
         <v>164</v>
       </c>
       <c r="B197" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
@@ -2499,6 +2473,54 @@
         <v>164</v>
       </c>
       <c r="B198" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>164</v>
+      </c>
+      <c r="B199" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>164</v>
+      </c>
+      <c r="B200" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>164</v>
+      </c>
+      <c r="B201" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>164</v>
+      </c>
+      <c r="B202" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>164</v>
+      </c>
+      <c r="B203" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>164</v>
+      </c>
+      <c r="B204" t="s">
         <v>184</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add more train word no 7
</commit_message>
<xml_diff>
--- a/data/train.xlsx
+++ b/data/train.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project_chatbot\chat_bot_team\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFC9CA6-BAAC-4E53-939E-FC6B46AAFBBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560AD53A-7856-42C9-84BF-D137E8329073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="202">
   <si>
     <t>tag</t>
   </si>
@@ -620,6 +620,12 @@
   </si>
   <si>
     <t>กฎหมายเกี่ยวกับลูกค้า</t>
+  </si>
+  <si>
+    <t>ขายอะไรแล้วติดคุก</t>
+  </si>
+  <si>
+    <t>อะไรที่ควรระวัง</t>
   </si>
 </sst>
 </file>
@@ -996,10 +1002,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B204"/>
+  <dimension ref="A1:B214"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="B108" sqref="B108"/>
+    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="B139" sqref="B139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2020,84 +2026,20 @@
         <v>122</v>
       </c>
     </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>98</v>
+      </c>
+      <c r="B138" t="s">
+        <v>200</v>
+      </c>
+    </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="B139" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>123</v>
-      </c>
-      <c r="B140" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>123</v>
-      </c>
-      <c r="B141" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>123</v>
-      </c>
-      <c r="B142" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>123</v>
-      </c>
-      <c r="B143" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>123</v>
-      </c>
-      <c r="B144" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>123</v>
-      </c>
-      <c r="B145" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>123</v>
-      </c>
-      <c r="B146" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
-        <v>123</v>
-      </c>
-      <c r="B147" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>123</v>
-      </c>
-      <c r="B148" t="s">
-        <v>130</v>
+        <v>201</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
@@ -2105,7 +2047,7 @@
         <v>123</v>
       </c>
       <c r="B149" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
@@ -2113,7 +2055,7 @@
         <v>123</v>
       </c>
       <c r="B150" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
@@ -2121,7 +2063,7 @@
         <v>123</v>
       </c>
       <c r="B151" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
@@ -2129,7 +2071,7 @@
         <v>123</v>
       </c>
       <c r="B152" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
@@ -2137,7 +2079,7 @@
         <v>123</v>
       </c>
       <c r="B153" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
@@ -2145,7 +2087,7 @@
         <v>123</v>
       </c>
       <c r="B154" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
@@ -2153,7 +2095,7 @@
         <v>123</v>
       </c>
       <c r="B155" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
@@ -2161,7 +2103,7 @@
         <v>123</v>
       </c>
       <c r="B156" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
@@ -2169,7 +2111,7 @@
         <v>123</v>
       </c>
       <c r="B157" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
@@ -2177,7 +2119,7 @@
         <v>123</v>
       </c>
       <c r="B158" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
@@ -2185,7 +2127,7 @@
         <v>123</v>
       </c>
       <c r="B159" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
@@ -2193,7 +2135,7 @@
         <v>123</v>
       </c>
       <c r="B160" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
@@ -2201,87 +2143,87 @@
         <v>123</v>
       </c>
       <c r="B161" t="s">
-        <v>144</v>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>123</v>
+      </c>
+      <c r="B162" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="B163" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="B164" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="B165" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="B166" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="B167" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="B168" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="B169" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="B170" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="B171" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
-        <v>145</v>
-      </c>
-      <c r="B172" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
@@ -2289,7 +2231,7 @@
         <v>145</v>
       </c>
       <c r="B173" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
@@ -2297,135 +2239,135 @@
         <v>145</v>
       </c>
       <c r="B174" t="s">
-        <v>157</v>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>145</v>
+      </c>
+      <c r="B175" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B176" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B177" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B178" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B179" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B180" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B181" t="s">
-        <v>185</v>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>145</v>
+      </c>
+      <c r="B182" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>186</v>
+        <v>145</v>
       </c>
       <c r="B183" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>186</v>
+        <v>145</v>
       </c>
       <c r="B184" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
-        <v>186</v>
-      </c>
-      <c r="B185" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>186</v>
+        <v>158</v>
       </c>
       <c r="B186" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>186</v>
+        <v>158</v>
       </c>
       <c r="B187" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>186</v>
+        <v>158</v>
       </c>
       <c r="B188" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>186</v>
+        <v>158</v>
       </c>
       <c r="B189" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>186</v>
+        <v>158</v>
       </c>
       <c r="B190" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>186</v>
+        <v>158</v>
       </c>
       <c r="B191" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
-        <v>186</v>
-      </c>
-      <c r="B192" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
@@ -2433,7 +2375,7 @@
         <v>186</v>
       </c>
       <c r="B193" t="s">
-        <v>187</v>
+        <v>165</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
@@ -2441,86 +2383,166 @@
         <v>186</v>
       </c>
       <c r="B194" t="s">
-        <v>188</v>
+        <v>166</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>164</v>
+        <v>186</v>
       </c>
       <c r="B195" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>164</v>
+        <v>186</v>
       </c>
       <c r="B196" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>164</v>
+        <v>186</v>
       </c>
       <c r="B197" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>164</v>
+        <v>186</v>
       </c>
       <c r="B198" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>164</v>
+        <v>186</v>
       </c>
       <c r="B199" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>164</v>
+        <v>186</v>
       </c>
       <c r="B200" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>164</v>
+        <v>186</v>
       </c>
       <c r="B201" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>164</v>
+        <v>186</v>
       </c>
       <c r="B202" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>164</v>
+        <v>186</v>
       </c>
       <c r="B203" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
+        <v>186</v>
+      </c>
+      <c r="B204" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
         <v>164</v>
       </c>
-      <c r="B204" t="s">
+      <c r="B205" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>164</v>
+      </c>
+      <c r="B206" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>164</v>
+      </c>
+      <c r="B207" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>164</v>
+      </c>
+      <c r="B208" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>164</v>
+      </c>
+      <c r="B209" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>164</v>
+      </c>
+      <c r="B210" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>164</v>
+      </c>
+      <c r="B211" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>164</v>
+      </c>
+      <c r="B212" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>164</v>
+      </c>
+      <c r="B213" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>164</v>
+      </c>
+      <c r="B214" t="s">
         <v>184</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add question for tag บอทโง่
</commit_message>
<xml_diff>
--- a/data/train.xlsx
+++ b/data/train.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B202"/>
+  <dimension ref="A1:B213"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -804,14 +804,6 @@
         <v>ขั้นตอน</v>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" t="str">
-        <v>สาม</v>
-      </c>
-      <c r="B59" t="str">
-        <v>จดทะเบียนยังไง</v>
-      </c>
-    </row>
     <row r="60">
       <c r="A60" t="str">
         <v>สี่</v>
@@ -986,14 +978,6 @@
       </c>
       <c r="B81" t="str">
         <v>เริ่มต้นขายออนไลน์</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="str">
-        <v>สี่</v>
-      </c>
-      <c r="B82" t="str">
-        <v>จะขายของนี้ต้องทำไรบ้าง</v>
       </c>
     </row>
     <row r="84">
@@ -1838,31 +1822,119 @@
     </row>
     <row r="200">
       <c r="A200" t="str">
-        <v>easter</v>
+        <v>บอทโง่</v>
       </c>
       <c r="B200" t="str">
-        <v>พี่โบ๊ท</v>
+        <v>ตอบผิด</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="str">
-        <v>easter</v>
+        <v>บอทโง่</v>
       </c>
       <c r="B201" t="str">
-        <v>อาจารย์โบ๊ท</v>
+        <v>ตอบไม่ตรง</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="str">
-        <v>easter</v>
+        <v>บอทโง่</v>
       </c>
       <c r="B202" t="str">
-        <v>จารย์โบ๊ท</v>
+        <v>ไม่น่าใช่</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="str">
+        <v>บอทโง่</v>
+      </c>
+      <c r="B203" t="str">
+        <v>ผิดเรื่อง</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="str">
+        <v>บอทโง่</v>
+      </c>
+      <c r="B204" t="str">
+        <v>ผิดประเด็น</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="str">
+        <v>บอทโง่</v>
+      </c>
+      <c r="B205" t="str">
+        <v>แปลกๆ</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="str">
+        <v>บอทโง่</v>
+      </c>
+      <c r="B206" t="str">
+        <v>งง</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="str">
+        <v>บอทโง่</v>
+      </c>
+      <c r="B207" t="str">
+        <v>ใช่หรอ</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="str">
+        <v>บอทโง่</v>
+      </c>
+      <c r="B208" t="str">
+        <v>ตอบผิดเปล่า</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="str">
+        <v>บอทโง่</v>
+      </c>
+      <c r="B209" t="str">
+        <v>ตอบไม่ตรงคำถาม</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="str">
+        <v>บอทโง่</v>
+      </c>
+      <c r="B210" t="str">
+        <v>นอกเรื่อง</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="str">
+        <v>บอทโง่</v>
+      </c>
+      <c r="B211" t="str">
+        <v>ไม่ใช่ละ</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="str">
+        <v>บอทโง่</v>
+      </c>
+      <c r="B212" t="str">
+        <v>ห้ะ</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="str">
+        <v>บอทโง่</v>
+      </c>
+      <c r="B213" t="str">
+        <v>ไรนะ</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B202"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B213"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add some question for each tag
</commit_message>
<xml_diff>
--- a/data/train.xlsx
+++ b/data/train.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B221"/>
+  <dimension ref="A1:B227"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1694,7 +1694,7 @@
     </row>
     <row r="177">
       <c r="A177" t="str">
-        <v>greet</v>
+        <v>ทักทาย</v>
       </c>
       <c r="B177" t="str">
         <v>Hello</v>
@@ -1702,7 +1702,7 @@
     </row>
     <row r="178">
       <c r="A178" t="str">
-        <v>greet</v>
+        <v>ทักทาย</v>
       </c>
       <c r="B178" t="str">
         <v>Hi</v>
@@ -1710,7 +1710,7 @@
     </row>
     <row r="179">
       <c r="A179" t="str">
-        <v>greet</v>
+        <v>ทักทาย</v>
       </c>
       <c r="B179" t="str">
         <v>Hey</v>
@@ -1718,7 +1718,7 @@
     </row>
     <row r="180">
       <c r="A180" t="str">
-        <v>greet</v>
+        <v>ทักทาย</v>
       </c>
       <c r="B180" t="str">
         <v>Yo</v>
@@ -1726,7 +1726,7 @@
     </row>
     <row r="181">
       <c r="A181" t="str">
-        <v>greet</v>
+        <v>ทักทาย</v>
       </c>
       <c r="B181" t="str">
         <v>Yep</v>
@@ -1734,7 +1734,7 @@
     </row>
     <row r="182">
       <c r="A182" t="str">
-        <v>greet</v>
+        <v>ทักทาย</v>
       </c>
       <c r="B182" t="str">
         <v>Sup</v>
@@ -1742,7 +1742,7 @@
     </row>
     <row r="183">
       <c r="A183" t="str">
-        <v>greet</v>
+        <v>ทักทาย</v>
       </c>
       <c r="B183" t="str">
         <v>What</v>
@@ -1750,7 +1750,7 @@
     </row>
     <row r="184">
       <c r="A184" t="str">
-        <v>greet</v>
+        <v>ทักทาย</v>
       </c>
       <c r="B184" t="str">
         <v>What's up</v>
@@ -1758,7 +1758,7 @@
     </row>
     <row r="185">
       <c r="A185" t="str">
-        <v>greet</v>
+        <v>ทักทาย</v>
       </c>
       <c r="B185" t="str">
         <v>Yea</v>
@@ -1766,7 +1766,7 @@
     </row>
     <row r="186">
       <c r="A186" t="str">
-        <v>greet</v>
+        <v>ทักทาย</v>
       </c>
       <c r="B186" t="str">
         <v>Yeah</v>
@@ -1774,7 +1774,7 @@
     </row>
     <row r="187">
       <c r="A187" t="str">
-        <v>greet</v>
+        <v>ทักทาย</v>
       </c>
       <c r="B187" t="str">
         <v>Yess</v>
@@ -1782,7 +1782,7 @@
     </row>
     <row r="188">
       <c r="A188" t="str">
-        <v>greet</v>
+        <v>ทักทาย</v>
       </c>
       <c r="B188" t="str">
         <v>Yes</v>
@@ -1866,6 +1866,14 @@
       </c>
       <c r="B198" t="str">
         <v>สวัสดีนาย</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="str">
+        <v>สบายดี</v>
+      </c>
+      <c r="B203" t="str">
+        <v>บายดีป่าว</v>
       </c>
     </row>
     <row r="204">
@@ -1996,9 +2004,49 @@
         <v>หัวข้อ</v>
       </c>
     </row>
+    <row r="223">
+      <c r="A223" t="str">
+        <v>บอกลา</v>
+      </c>
+      <c r="B223" t="str">
+        <v>บาย</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="str">
+        <v>บอกลา</v>
+      </c>
+      <c r="B224" t="str">
+        <v>บ๊าย</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="str">
+        <v>บอกลา</v>
+      </c>
+      <c r="B225" t="str">
+        <v>บ้าย</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="str">
+        <v>บอกลา</v>
+      </c>
+      <c r="B226" t="str">
+        <v>ลาก่อน</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="str">
+        <v>บอกลา</v>
+      </c>
+      <c r="B227" t="str">
+        <v>ไว้เจอกันใหม่</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B221"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B227"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
create new keyword tag
</commit_message>
<xml_diff>
--- a/data/train.xlsx
+++ b/data/train.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Projects\baisd\chat_bot_team\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project_chatbot\chat_bot_team\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{572649EC-8558-487E-B0DD-7FE233ADEA23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA072F9E-D837-4497-AC1C-4CB79BA1B337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="244">
   <si>
     <t>tag</t>
   </si>
@@ -734,6 +734,24 @@
   </si>
   <si>
     <t>ถาม</t>
+  </si>
+  <si>
+    <t>เบื่อ</t>
+  </si>
+  <si>
+    <t>เบื่อจัง</t>
+  </si>
+  <si>
+    <t>เบื่อๆ</t>
+  </si>
+  <si>
+    <t>เหงา</t>
+  </si>
+  <si>
+    <t>เหงาๆ</t>
+  </si>
+  <si>
+    <t>เหงาจัง</t>
   </si>
 </sst>
 </file>
@@ -1110,15 +1128,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B241"/>
+  <dimension ref="A1:B248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A223" workbookViewId="0">
-      <selection activeCell="E244" sqref="E244"/>
+    <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
+      <selection activeCell="C243" sqref="C243"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1126,7 +1144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1134,7 +1152,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1142,7 +1160,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1150,7 +1168,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1158,7 +1176,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1166,7 +1184,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1174,7 +1192,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1182,7 +1200,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1190,7 +1208,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -1198,7 +1216,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -1206,7 +1224,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -1214,7 +1232,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1222,7 +1240,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1230,7 +1248,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -1238,7 +1256,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -1246,7 +1264,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -1254,7 +1272,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -1262,7 +1280,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -1270,7 +1288,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -1278,7 +1296,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -1286,7 +1304,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -1294,7 +1312,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>14</v>
       </c>
@@ -1302,7 +1320,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -1310,7 +1328,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -1318,7 +1336,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -1326,7 +1344,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -1334,7 +1352,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -1342,7 +1360,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>14</v>
       </c>
@@ -1350,7 +1368,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -1358,7 +1376,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>14</v>
       </c>
@@ -1366,7 +1384,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -1374,7 +1392,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -1382,7 +1400,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -1390,7 +1408,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>14</v>
       </c>
@@ -1398,7 +1416,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -1406,7 +1424,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -1414,7 +1432,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -1422,7 +1440,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>14</v>
       </c>
@@ -1430,7 +1448,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -1438,7 +1456,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -1446,7 +1464,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>42</v>
       </c>
@@ -1454,7 +1472,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>42</v>
       </c>
@@ -1462,7 +1480,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>42</v>
       </c>
@@ -1470,7 +1488,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>42</v>
       </c>
@@ -1478,7 +1496,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>42</v>
       </c>
@@ -1486,7 +1504,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>42</v>
       </c>
@@ -1494,7 +1512,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>42</v>
       </c>
@@ -1502,7 +1520,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>42</v>
       </c>
@@ -1510,7 +1528,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>42</v>
       </c>
@@ -1518,7 +1536,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>42</v>
       </c>
@@ -1526,7 +1544,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>42</v>
       </c>
@@ -1534,7 +1552,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>42</v>
       </c>
@@ -1542,7 +1560,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>42</v>
       </c>
@@ -1550,7 +1568,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>42</v>
       </c>
@@ -1558,7 +1576,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>42</v>
       </c>
@@ -1566,7 +1584,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>60</v>
       </c>
@@ -1574,7 +1592,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -1582,7 +1600,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -1590,7 +1608,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>60</v>
       </c>
@@ -1598,7 +1616,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>60</v>
       </c>
@@ -1606,7 +1624,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>60</v>
       </c>
@@ -1614,7 +1632,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>60</v>
       </c>
@@ -1622,7 +1640,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>60</v>
       </c>
@@ -1630,7 +1648,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>60</v>
       </c>
@@ -1638,7 +1656,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>60</v>
       </c>
@@ -1646,7 +1664,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>60</v>
       </c>
@@ -1654,7 +1672,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>60</v>
       </c>
@@ -1662,7 +1680,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>60</v>
       </c>
@@ -1670,7 +1688,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>60</v>
       </c>
@@ -1678,7 +1696,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>60</v>
       </c>
@@ -1686,7 +1704,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>60</v>
       </c>
@@ -1694,7 +1712,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>60</v>
       </c>
@@ -1702,7 +1720,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>60</v>
       </c>
@@ -1710,7 +1728,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>60</v>
       </c>
@@ -1718,7 +1736,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>60</v>
       </c>
@@ -1726,7 +1744,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>60</v>
       </c>
@@ -1734,7 +1752,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>60</v>
       </c>
@@ -1742,7 +1760,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>60</v>
       </c>
@@ -1750,7 +1768,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>60</v>
       </c>
@@ -1758,7 +1776,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>85</v>
       </c>
@@ -1766,7 +1784,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>85</v>
       </c>
@@ -1774,7 +1792,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>85</v>
       </c>
@@ -1782,7 +1800,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>85</v>
       </c>
@@ -1790,7 +1808,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>85</v>
       </c>
@@ -1798,7 +1816,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>85</v>
       </c>
@@ -1806,7 +1824,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>85</v>
       </c>
@@ -1814,7 +1832,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>85</v>
       </c>
@@ -1822,7 +1840,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>85</v>
       </c>
@@ -1830,7 +1848,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>95</v>
       </c>
@@ -1838,7 +1856,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>95</v>
       </c>
@@ -1846,7 +1864,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>95</v>
       </c>
@@ -1854,7 +1872,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>95</v>
       </c>
@@ -1862,7 +1880,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>95</v>
       </c>
@@ -1870,7 +1888,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>95</v>
       </c>
@@ -1878,7 +1896,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>95</v>
       </c>
@@ -1886,7 +1904,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>95</v>
       </c>
@@ -1894,7 +1912,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>104</v>
       </c>
@@ -1902,7 +1920,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>104</v>
       </c>
@@ -1910,7 +1928,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>104</v>
       </c>
@@ -1918,7 +1936,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>104</v>
       </c>
@@ -1926,7 +1944,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>104</v>
       </c>
@@ -1934,7 +1952,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>104</v>
       </c>
@@ -1942,7 +1960,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>104</v>
       </c>
@@ -1950,7 +1968,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>104</v>
       </c>
@@ -1958,7 +1976,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>104</v>
       </c>
@@ -1966,7 +1984,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>104</v>
       </c>
@@ -1974,7 +1992,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>104</v>
       </c>
@@ -1982,7 +2000,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>104</v>
       </c>
@@ -1990,7 +2008,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>104</v>
       </c>
@@ -1998,7 +2016,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>104</v>
       </c>
@@ -2006,7 +2024,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>104</v>
       </c>
@@ -2014,7 +2032,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>104</v>
       </c>
@@ -2022,7 +2040,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>104</v>
       </c>
@@ -2030,7 +2048,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="124" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>104</v>
       </c>
@@ -2038,7 +2056,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="125" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>104</v>
       </c>
@@ -2046,7 +2064,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="126" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>104</v>
       </c>
@@ -2054,7 +2072,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="127" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>104</v>
       </c>
@@ -2062,7 +2080,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="128" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>104</v>
       </c>
@@ -2070,7 +2088,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>104</v>
       </c>
@@ -2078,7 +2096,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>104</v>
       </c>
@@ -2086,7 +2104,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="131" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>104</v>
       </c>
@@ -2094,7 +2112,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="133" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>129</v>
       </c>
@@ -2102,7 +2120,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="134" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>129</v>
       </c>
@@ -2110,7 +2128,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="135" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>129</v>
       </c>
@@ -2118,7 +2136,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="136" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>129</v>
       </c>
@@ -2126,7 +2144,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="137" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>129</v>
       </c>
@@ -2134,7 +2152,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="138" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>129</v>
       </c>
@@ -2142,7 +2160,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="139" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>129</v>
       </c>
@@ -2150,7 +2168,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="140" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>129</v>
       </c>
@@ -2158,7 +2176,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="141" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>129</v>
       </c>
@@ -2166,7 +2184,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="142" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>129</v>
       </c>
@@ -2174,7 +2192,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="143" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>129</v>
       </c>
@@ -2182,7 +2200,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="144" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>129</v>
       </c>
@@ -2190,7 +2208,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>129</v>
       </c>
@@ -2198,7 +2216,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="146" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>129</v>
       </c>
@@ -2206,7 +2224,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="147" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>129</v>
       </c>
@@ -2214,7 +2232,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="148" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>129</v>
       </c>
@@ -2222,7 +2240,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="149" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>129</v>
       </c>
@@ -2230,7 +2248,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="150" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>129</v>
       </c>
@@ -2238,7 +2256,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>129</v>
       </c>
@@ -2246,7 +2264,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>129</v>
       </c>
@@ -2254,7 +2272,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>129</v>
       </c>
@@ -2262,7 +2280,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="154" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>129</v>
       </c>
@@ -2270,7 +2288,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="155" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>129</v>
       </c>
@@ -2278,7 +2296,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="157" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>151</v>
       </c>
@@ -2286,7 +2304,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="158" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>151</v>
       </c>
@@ -2294,7 +2312,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="159" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>151</v>
       </c>
@@ -2302,7 +2320,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="160" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>151</v>
       </c>
@@ -2310,7 +2328,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="161" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>151</v>
       </c>
@@ -2318,7 +2336,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="162" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>151</v>
       </c>
@@ -2326,7 +2344,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="163" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>151</v>
       </c>
@@ -2334,7 +2352,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="164" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>151</v>
       </c>
@@ -2342,7 +2360,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="165" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>151</v>
       </c>
@@ -2350,7 +2368,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="166" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>151</v>
       </c>
@@ -2358,7 +2376,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="167" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>151</v>
       </c>
@@ -2366,7 +2384,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>151</v>
       </c>
@@ -2374,7 +2392,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="170" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>164</v>
       </c>
@@ -2382,7 +2400,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="171" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>164</v>
       </c>
@@ -2390,7 +2408,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="172" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>164</v>
       </c>
@@ -2398,7 +2416,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="173" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>164</v>
       </c>
@@ -2406,7 +2424,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="174" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>164</v>
       </c>
@@ -2414,7 +2432,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="175" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>164</v>
       </c>
@@ -2422,7 +2440,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="176" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>164</v>
       </c>
@@ -2430,7 +2448,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="177" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>172</v>
       </c>
@@ -2438,7 +2456,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="178" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>172</v>
       </c>
@@ -2446,7 +2464,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="179" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>172</v>
       </c>
@@ -2454,7 +2472,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="180" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>172</v>
       </c>
@@ -2462,7 +2480,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="181" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>172</v>
       </c>
@@ -2470,7 +2488,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="182" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>172</v>
       </c>
@@ -2478,7 +2496,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="183" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>172</v>
       </c>
@@ -2486,7 +2504,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="184" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>172</v>
       </c>
@@ -2494,7 +2512,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="185" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>172</v>
       </c>
@@ -2502,7 +2520,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="186" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>172</v>
       </c>
@@ -2510,7 +2528,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="187" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>172</v>
       </c>
@@ -2518,7 +2536,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="188" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>172</v>
       </c>
@@ -2526,7 +2544,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>172</v>
       </c>
@@ -2534,7 +2552,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>172</v>
       </c>
@@ -2542,7 +2560,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="191" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>172</v>
       </c>
@@ -2550,7 +2568,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="192" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>172</v>
       </c>
@@ -2558,7 +2576,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="193" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>172</v>
       </c>
@@ -2566,7 +2584,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="194" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>172</v>
       </c>
@@ -2574,7 +2592,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="195" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>172</v>
       </c>
@@ -2582,7 +2600,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="196" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>172</v>
       </c>
@@ -2590,7 +2608,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="197" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>172</v>
       </c>
@@ -2598,7 +2616,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>172</v>
       </c>
@@ -2606,7 +2624,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>172</v>
       </c>
@@ -2614,7 +2632,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>172</v>
       </c>
@@ -2622,7 +2640,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>172</v>
       </c>
@@ -2630,7 +2648,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>172</v>
       </c>
@@ -2638,7 +2656,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="203" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>195</v>
       </c>
@@ -2646,7 +2664,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="204" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>195</v>
       </c>
@@ -2654,7 +2672,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="205" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>195</v>
       </c>
@@ -2662,7 +2680,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="206" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>195</v>
       </c>
@@ -2670,7 +2688,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="208" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>200</v>
       </c>
@@ -2678,7 +2696,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="209" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>200</v>
       </c>
@@ -2686,7 +2704,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="210" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>200</v>
       </c>
@@ -2694,8 +2712,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="211" spans="1:2" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="212" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>204</v>
       </c>
@@ -2703,7 +2720,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="213" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>204</v>
       </c>
@@ -2711,7 +2728,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="214" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>204</v>
       </c>
@@ -2719,7 +2736,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="215" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>208</v>
       </c>
@@ -2727,7 +2744,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="216" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>208</v>
       </c>
@@ -2735,7 +2752,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="217" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>211</v>
       </c>
@@ -2743,7 +2760,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="218" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>211</v>
       </c>
@@ -2751,7 +2768,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="220" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>213</v>
       </c>
@@ -2759,7 +2776,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="221" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>213</v>
       </c>
@@ -2767,7 +2784,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="223" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>215</v>
       </c>
@@ -2775,7 +2792,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="224" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>215</v>
       </c>
@@ -2783,7 +2800,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="225" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>215</v>
       </c>
@@ -2791,7 +2808,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="226" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>215</v>
       </c>
@@ -2799,7 +2816,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="227" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>215</v>
       </c>
@@ -2807,7 +2824,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>225</v>
       </c>
@@ -2815,7 +2832,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>225</v>
       </c>
@@ -2823,7 +2840,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>225</v>
       </c>
@@ -2831,7 +2848,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>225</v>
       </c>
@@ -2839,7 +2856,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>225</v>
       </c>
@@ -2847,7 +2864,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>225</v>
       </c>
@@ -2855,7 +2872,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>232</v>
       </c>
@@ -2863,7 +2880,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>232</v>
       </c>
@@ -2871,7 +2888,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>232</v>
       </c>
@@ -2879,7 +2896,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>232</v>
       </c>
@@ -2887,7 +2904,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>232</v>
       </c>
@@ -2895,12 +2912,60 @@
         <v>236</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>232</v>
       </c>
       <c r="B241" t="s">
         <v>237</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>238</v>
+      </c>
+      <c r="B243" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>238</v>
+      </c>
+      <c r="B244" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>238</v>
+      </c>
+      <c r="B245" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>238</v>
+      </c>
+      <c r="B246" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>238</v>
+      </c>
+      <c r="B247" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>238</v>
+      </c>
+      <c r="B248" t="s">
+        <v>243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create new tag keywords
</commit_message>
<xml_diff>
--- a/data/train.xlsx
+++ b/data/train.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project_chatbot\chat_bot_team\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA072F9E-D837-4497-AC1C-4CB79BA1B337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B473C5C-D3BE-49D7-8950-92C9C8875CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="254">
   <si>
     <t>tag</t>
   </si>
@@ -752,6 +752,36 @@
   </si>
   <si>
     <t>เหงาจัง</t>
+  </si>
+  <si>
+    <t>ตกลง</t>
+  </si>
+  <si>
+    <t>โอเค</t>
+  </si>
+  <si>
+    <t>เค</t>
+  </si>
+  <si>
+    <t>เคร</t>
+  </si>
+  <si>
+    <t>ได้</t>
+  </si>
+  <si>
+    <t>โอเช</t>
+  </si>
+  <si>
+    <t>เค้</t>
+  </si>
+  <si>
+    <t>เค๊</t>
+  </si>
+  <si>
+    <t>ถูกหนึ่ง</t>
+  </si>
+  <si>
+    <t>ประเทศไทย เพราะไทยมีตรัง</t>
   </si>
 </sst>
 </file>
@@ -1128,10 +1158,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B248"/>
+  <dimension ref="A1:B258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
-      <selection activeCell="C243" sqref="C243"/>
+    <sheetView tabSelected="1" topLeftCell="A247" workbookViewId="0">
+      <selection activeCell="A259" sqref="A259"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2968,6 +2998,78 @@
         <v>243</v>
       </c>
     </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>244</v>
+      </c>
+      <c r="B250" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>244</v>
+      </c>
+      <c r="B251" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>244</v>
+      </c>
+      <c r="B252" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>244</v>
+      </c>
+      <c r="B253" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>244</v>
+      </c>
+      <c r="B254" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>244</v>
+      </c>
+      <c r="B255" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>244</v>
+      </c>
+      <c r="B256" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>244</v>
+      </c>
+      <c r="B257" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>252</v>
+      </c>
+      <c r="B258" t="s">
+        <v>253</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
add more train word
</commit_message>
<xml_diff>
--- a/data/train.xlsx
+++ b/data/train.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project_chatbot\chat_bot_team\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B66A8AD0-1B7A-4BAB-A16A-F3B63FCAA5C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F4999F-9737-4B0B-A07B-0EF85BF5D010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="260">
   <si>
     <t>tag</t>
   </si>
@@ -784,13 +784,22 @@
     <t>โอเคร</t>
   </si>
   <si>
-    <t>ประเทศไทย เพราะประเทศไทยมีตรัง (ตัง)</t>
-  </si>
-  <si>
     <t>ถูกสอง</t>
   </si>
   <si>
     <t>ไปฉันเพล</t>
+  </si>
+  <si>
+    <t>ไทย</t>
+  </si>
+  <si>
+    <t>ตรัง</t>
+  </si>
+  <si>
+    <t>ประเทศไทย เพราะประเทศไทยมีตรัง</t>
+  </si>
+  <si>
+    <t>ไทย เพราะประเทศไทยมีตรัง</t>
   </si>
 </sst>
 </file>
@@ -1167,10 +1176,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B260"/>
+  <dimension ref="A1:B264"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A247" workbookViewId="0">
-      <selection activeCell="B260" sqref="B260"/>
+      <selection activeCell="C269" sqref="C269"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3084,15 +3093,39 @@
         <v>252</v>
       </c>
       <c r="B259" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
+        <v>252</v>
+      </c>
+      <c r="B260" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>252</v>
+      </c>
+      <c r="B261" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>252</v>
+      </c>
+      <c r="B262" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>254</v>
+      </c>
+      <c r="B264" t="s">
         <v>255</v>
-      </c>
-      <c r="B260" t="s">
-        <v>256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add more word train
</commit_message>
<xml_diff>
--- a/data/train.xlsx
+++ b/data/train.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project_chatbot\chat_bot_team\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F4999F-9737-4B0B-A07B-0EF85BF5D010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EBFAD42-CECB-46DD-99B7-99C58EB65285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="265">
   <si>
     <t>tag</t>
   </si>
@@ -800,6 +800,21 @@
   </si>
   <si>
     <t>ไทย เพราะประเทศไทยมีตรัง</t>
+  </si>
+  <si>
+    <t>ไทย เพราะมีตรัง</t>
+  </si>
+  <si>
+    <t>ประเทศไทย เพราะมีตรัง</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>okay</t>
   </si>
 </sst>
 </file>
@@ -1176,10 +1191,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B264"/>
+  <dimension ref="A1:B270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A247" workbookViewId="0">
-      <selection activeCell="C269" sqref="C269"/>
+    <sheetView tabSelected="1" topLeftCell="A253" workbookViewId="0">
+      <selection activeCell="E266" sqref="E266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3090,41 +3105,81 @@
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="B259" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="B260" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
+        <v>244</v>
+      </c>
+      <c r="B261" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
         <v>252</v>
       </c>
-      <c r="B261" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A262" t="s">
-        <v>252</v>
-      </c>
-      <c r="B262" t="s">
-        <v>257</v>
+      <c r="B263" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
+        <v>252</v>
+      </c>
+      <c r="B264" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>252</v>
+      </c>
+      <c r="B265" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>252</v>
+      </c>
+      <c r="B266" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>252</v>
+      </c>
+      <c r="B267" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>252</v>
+      </c>
+      <c r="B268" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
         <v>254</v>
       </c>
-      <c r="B264" t="s">
+      <c r="B270" t="s">
         <v>255</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add more train words
</commit_message>
<xml_diff>
--- a/data/train.xlsx
+++ b/data/train.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project_chatbot\chat_bot_team\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EBFAD42-CECB-46DD-99B7-99C58EB65285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6329E133-7364-4FA6-95C8-919B029F900D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="267">
   <si>
     <t>tag</t>
   </si>
@@ -815,6 +815,12 @@
   </si>
   <si>
     <t>okay</t>
+  </si>
+  <si>
+    <t>ฉันเพล</t>
+  </si>
+  <si>
+    <t>ฉันข้าว</t>
   </si>
 </sst>
 </file>
@@ -1191,10 +1197,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B270"/>
+  <dimension ref="A1:B274"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A253" workbookViewId="0">
-      <selection activeCell="E266" sqref="E266"/>
+      <selection activeCell="B274" sqref="B274"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3183,6 +3189,38 @@
         <v>255</v>
       </c>
     </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>254</v>
+      </c>
+      <c r="B271" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>254</v>
+      </c>
+      <c r="B272" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>254</v>
+      </c>
+      <c r="B273" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>254</v>
+      </c>
+      <c r="B274" t="s">
+        <v>266</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
create new tag and add keyword train
</commit_message>
<xml_diff>
--- a/data/train.xlsx
+++ b/data/train.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project_chatbot\chat_bot_team\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6329E133-7364-4FA6-95C8-919B029F900D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5444BC-36BD-4807-85C2-65ACDD5E7632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="274">
   <si>
     <t>tag</t>
   </si>
@@ -821,6 +821,27 @@
   </si>
   <si>
     <t>ฉันข้าว</t>
+  </si>
+  <si>
+    <t>ถูกสาม</t>
+  </si>
+  <si>
+    <t>ปีโป้</t>
+  </si>
+  <si>
+    <t>ปีโป๊</t>
+  </si>
+  <si>
+    <t>ปีโป้หลากสี</t>
+  </si>
+  <si>
+    <t>ปีปีโป้ปะปะปีปีโป้</t>
+  </si>
+  <si>
+    <t>ปีโป้ไง</t>
+  </si>
+  <si>
+    <t>ปีโป้ครับ</t>
   </si>
 </sst>
 </file>
@@ -1197,10 +1218,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B274"/>
+  <dimension ref="A1:B281"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A253" workbookViewId="0">
-      <selection activeCell="B274" sqref="B274"/>
+    <sheetView tabSelected="1" topLeftCell="A265" workbookViewId="0">
+      <selection activeCell="B281" sqref="B281"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3221,6 +3242,54 @@
         <v>266</v>
       </c>
     </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>267</v>
+      </c>
+      <c r="B276" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>267</v>
+      </c>
+      <c r="B277" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>267</v>
+      </c>
+      <c r="B278" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>267</v>
+      </c>
+      <c r="B279" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>267</v>
+      </c>
+      <c r="B280" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>267</v>
+      </c>
+      <c r="B281" t="s">
+        <v>273</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
add more train phrase
</commit_message>
<xml_diff>
--- a/data/train.xlsx
+++ b/data/train.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project_chatbot\chat_bot_team\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5444BC-36BD-4807-85C2-65ACDD5E7632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8374C4E-A4F1-44CB-BA6A-6887D88C5D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="279">
   <si>
     <t>tag</t>
   </si>
@@ -842,6 +842,21 @@
   </si>
   <si>
     <t>ปีโป้ครับ</t>
+  </si>
+  <si>
+    <t>ทำไร</t>
+  </si>
+  <si>
+    <t>ทำไรอะ</t>
+  </si>
+  <si>
+    <t>ทำไรอยู่</t>
+  </si>
+  <si>
+    <t>ทำอะไรอยู่ครับ</t>
+  </si>
+  <si>
+    <t>ทำอะไรอยู่คะ</t>
   </si>
 </sst>
 </file>
@@ -1218,10 +1233,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B281"/>
+  <dimension ref="A1:B286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A265" workbookViewId="0">
-      <selection activeCell="B281" sqref="B281"/>
+    <sheetView tabSelected="1" topLeftCell="A209" workbookViewId="0">
+      <selection activeCell="A224" sqref="A224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2844,114 +2859,114 @@
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B217" t="s">
-        <v>211</v>
+        <v>274</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B218" t="s">
-        <v>212</v>
+        <v>276</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>208</v>
+      </c>
+      <c r="B219" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B220" t="s">
-        <v>214</v>
+        <v>277</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B221" t="s">
-        <v>213</v>
+        <v>278</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>211</v>
+      </c>
+      <c r="B222" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B223" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A224" t="s">
-        <v>215</v>
-      </c>
-      <c r="B224" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B225" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
+        <v>213</v>
+      </c>
+      <c r="B226" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
         <v>215</v>
       </c>
-      <c r="B226" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A227" t="s">
-        <v>215</v>
-      </c>
-      <c r="B227" t="s">
-        <v>220</v>
+      <c r="B228" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="B229" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="B230" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="B231" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="B232" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A233" t="s">
-        <v>225</v>
-      </c>
-      <c r="B233" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
@@ -2959,47 +2974,47 @@
         <v>225</v>
       </c>
       <c r="B234" t="s">
-        <v>231</v>
+        <v>226</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>225</v>
+      </c>
+      <c r="B235" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="B236" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="B237" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="B238" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="B239" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A240" t="s">
-        <v>232</v>
-      </c>
-      <c r="B240" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
@@ -3007,47 +3022,47 @@
         <v>232</v>
       </c>
       <c r="B241" t="s">
-        <v>237</v>
+        <v>232</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>232</v>
+      </c>
+      <c r="B242" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="B243" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="B244" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="B245" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="B246" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A247" t="s">
-        <v>238</v>
-      </c>
-      <c r="B247" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
@@ -3055,47 +3070,47 @@
         <v>238</v>
       </c>
       <c r="B248" t="s">
-        <v>243</v>
+        <v>238</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>238</v>
+      </c>
+      <c r="B249" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="B250" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="B251" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="B252" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="B253" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A254" t="s">
-        <v>244</v>
-      </c>
-      <c r="B254" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
@@ -3103,7 +3118,7 @@
         <v>244</v>
       </c>
       <c r="B255" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
@@ -3111,7 +3126,7 @@
         <v>244</v>
       </c>
       <c r="B256" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
@@ -3119,7 +3134,7 @@
         <v>244</v>
       </c>
       <c r="B257" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
@@ -3127,7 +3142,7 @@
         <v>244</v>
       </c>
       <c r="B258" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
@@ -3135,7 +3150,7 @@
         <v>244</v>
       </c>
       <c r="B259" t="s">
-        <v>262</v>
+        <v>244</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
@@ -3143,7 +3158,7 @@
         <v>244</v>
       </c>
       <c r="B260" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
@@ -3151,47 +3166,47 @@
         <v>244</v>
       </c>
       <c r="B261" t="s">
-        <v>264</v>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>244</v>
+      </c>
+      <c r="B262" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="B263" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="B264" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="B265" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="B266" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A267" t="s">
-        <v>252</v>
-      </c>
-      <c r="B267" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
@@ -3199,87 +3214,87 @@
         <v>252</v>
       </c>
       <c r="B268" t="s">
-        <v>257</v>
+        <v>258</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>252</v>
+      </c>
+      <c r="B269" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B270" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B271" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B272" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
+        <v>252</v>
+      </c>
+      <c r="B273" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
         <v>254</v>
       </c>
-      <c r="B273" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A274" t="s">
-        <v>254</v>
-      </c>
-      <c r="B274" t="s">
-        <v>266</v>
+      <c r="B275" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="B276" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="B277" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="B278" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="B279" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A280" t="s">
-        <v>267</v>
-      </c>
-      <c r="B280" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
@@ -3287,13 +3302,53 @@
         <v>267</v>
       </c>
       <c r="B281" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>267</v>
+      </c>
+      <c r="B282" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>267</v>
+      </c>
+      <c r="B283" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>267</v>
+      </c>
+      <c r="B284" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>267</v>
+      </c>
+      <c r="B285" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>267</v>
+      </c>
+      <c r="B286" t="s">
         <v>273</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:B198 A203:B210 A212:B227" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:B198 A203:B210 A212:B216" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add question tag where
</commit_message>
<xml_diff>
--- a/data/train.xlsx
+++ b/data/train.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B316"/>
+  <dimension ref="A1:B322"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2724,9 +2724,49 @@
         <v>อากาศเป็นยังไง</v>
       </c>
     </row>
+    <row r="318">
+      <c r="A318" t="str">
+        <v>where</v>
+      </c>
+      <c r="B318" t="str">
+        <v>where are you?</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="str">
+        <v>where</v>
+      </c>
+      <c r="B319" t="str">
+        <v>Where are you?</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="str">
+        <v>where</v>
+      </c>
+      <c r="B320" t="str">
+        <v>where are you from?</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="str">
+        <v>where</v>
+      </c>
+      <c r="B321" t="str">
+        <v>Where are u from</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="str">
+        <v>where</v>
+      </c>
+      <c r="B322" t="str">
+        <v>where are u</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B316"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B322"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>